<commit_message>
Bar + Donut Chart with error handling
</commit_message>
<xml_diff>
--- a/SMIF Portfolio Tracker.xlsx
+++ b/SMIF Portfolio Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\smifwebsite\ausmif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D152E28-4732-4811-A81B-2C1F976A345D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0242E480-D15D-4DCD-BBB6-75A2323C6D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{8E62F0BB-DFF5-DE4B-9250-929F546166A9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="1" xr2:uid="{8E62F0BB-DFF5-DE4B-9250-929F546166A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="5" r:id="rId1"/>
@@ -1988,10 +1988,64 @@
     <v t="i">0</v>
   </a>
   <a r="1">
-    <v>159.26</v>
+    <v>234.79</v>
   </a>
   <a r="1">
-    <v>159.97</v>
+    <v>53.0961</v>
+  </a>
+  <a r="1">
+    <v>106.55</v>
+  </a>
+  <a r="1">
+    <v>472.65</v>
+  </a>
+  <a r="1">
+    <v>327</v>
+  </a>
+  <a r="1">
+    <v>185.64</v>
+  </a>
+  <a r="1">
+    <v>345.08</v>
+  </a>
+  <a r="1">
+    <v>139.56</v>
+  </a>
+  <a r="1">
+    <v>650.65</v>
+  </a>
+  <a r="1">
+    <v>149.93</v>
+  </a>
+  <a r="1">
+    <v>370.87</v>
+  </a>
+  <a r="1">
+    <v>456.12</v>
+  </a>
+  <a r="1">
+    <v>143.81</v>
+  </a>
+  <a r="1">
+    <v>209</v>
+  </a>
+  <a r="1">
+    <v>61.57</v>
+  </a>
+  <a r="1">
+    <v>11.54</v>
+  </a>
+  <a r="1">
+    <v>292.70999999999998</v>
+  </a>
+  <a r="1">
+    <v>81.45</v>
+  </a>
+  <a r="1">
+    <v>23.05</v>
+  </a>
+  <a r="1">
+    <v>233.42</v>
   </a>
   <a r="1">
     <v>189.12</v>
@@ -2003,73 +2057,19 @@
     <v>81.02</v>
   </a>
   <a r="1">
+    <v>159.26</v>
+  </a>
+  <a r="1">
     <v>580.07000000000005</v>
   </a>
   <a r="1">
-    <v>472.65</v>
-  </a>
-  <a r="1">
-    <v>327</v>
-  </a>
-  <a r="1">
-    <v>90.71</v>
-  </a>
-  <a r="1">
-    <v>456.12</v>
-  </a>
-  <a r="1">
-    <v>149.93</v>
-  </a>
-  <a r="1">
-    <v>370.87</v>
-  </a>
-  <a r="1">
-    <v>234.79</v>
-  </a>
-  <a r="1">
-    <v>53.0961</v>
-  </a>
-  <a r="1">
-    <v>81.45</v>
-  </a>
-  <a r="1">
-    <v>233.42</v>
-  </a>
-  <a r="1">
-    <v>185.64</v>
-  </a>
-  <a r="1">
-    <v>143.81</v>
-  </a>
-  <a r="1">
-    <v>650.65</v>
+    <v>159.97</v>
   </a>
   <a r="1">
     <v>421.89</v>
   </a>
   <a r="1">
-    <v>61.57</v>
-  </a>
-  <a r="1">
-    <v>23.05</v>
-  </a>
-  <a r="1">
-    <v>209</v>
-  </a>
-  <a r="1">
-    <v>139.56</v>
-  </a>
-  <a r="1">
-    <v>345.08</v>
-  </a>
-  <a r="1">
-    <v>106.55</v>
-  </a>
-  <a r="1">
-    <v>292.70999999999998</v>
-  </a>
-  <a r="1">
-    <v>11.54</v>
+    <v>90.71</v>
   </a>
 </arrayData>
 </file>
@@ -2098,11 +2098,11 @@
     <v>4</v>
     <v>260.10000000000002</v>
     <v>164.07499999999999</v>
-    <v>1.2093</v>
-    <v>0.49</v>
-    <v>-1.4010000000000001E-3</v>
-    <v>2.0230000000000001E-3</v>
-    <v>-0.34</v>
+    <v>1.1996</v>
+    <v>-7.99</v>
+    <v>4.7799999999999995E-3</v>
+    <v>-3.3856000000000004E-2</v>
+    <v>1.0900000000000001</v>
     <v>USD</v>
     <v>Apple Inc. designs, manufactures and markets smartphones, personal computers, tablets, wearables and accessories, and sells a variety of related services. Its product categories include iPhone, Mac, iPad, and Wearables, Home and Accessories. Its software platforms include iOS, iPadOS, macOS, watchOS, visionOS, and tvOS. Its services include advertising, AppleCare, cloud services, digital content and payment services. The Company operates various platforms, including the App Store, that allow customers to discover and download applications and digital content, such as books, music, video, games and podcasts. It also offers digital content through subscription-based services, including Apple Arcade, Apple Fitness+, Apple Music, Apple News+, and Apple TV+. Its products include iPhone 16 Pro, iPhone 16, iPhone 15, iPhone 14, iPhone SE, MacBook Air, MacBook Pro, iMac, Mac mini, Mac Studio, Mac Pro, iPad Pro, iPad Air, AirPods, AirPods Pro, AirPods Max, Apple TV and Apple Vision Pro.</v>
     <v>164000</v>
@@ -2110,25 +2110,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>One Apple Park Way, CUPERTINO, CA, 95014 US</v>
-    <v>243.7123</v>
+    <v>231.83</v>
     <v>Computers, Phones &amp; Household Electronics</v>
     <v>Stock</v>
-    <v>45666.041612939065</v>
+    <v>45691.912167291404</v>
     <v>1</v>
-    <v>240.05</v>
-    <v>3668609514000</v>
+    <v>225.7</v>
+    <v>3428784738700</v>
     <v>APPLE INC.</v>
     <v>APPLE INC.</v>
-    <v>241.92</v>
-    <v>39.903300000000002</v>
-    <v>242.21</v>
-    <v>242.7</v>
-    <v>242.36</v>
-    <v>15115820000</v>
+    <v>229.99</v>
+    <v>33.895400000000002</v>
+    <v>236</v>
+    <v>228.01</v>
+    <v>229.1</v>
+    <v>15037870000</v>
     <v>AAPL</v>
     <v>APPLE INC. (XNAS:AAPL)</v>
-    <v>37628940</v>
-    <v>46393136</v>
+    <v>72276419</v>
+    <v>54727315</v>
     <v>1977</v>
   </rv>
   <rv s="3">
@@ -2170,40 +2170,40 @@
     <v>8</v>
     <v>Finance</v>
     <v>4</v>
-    <v>638.25</v>
-    <v>415.51</v>
-    <v>1.3172999999999999</v>
-    <v>-3.05</v>
-    <v>-2.0019999999999999E-3</v>
-    <v>-7.2170000000000003E-3</v>
-    <v>-0.84</v>
+    <v>634.58989999999994</v>
+    <v>403.75</v>
+    <v>1.3126</v>
+    <v>1.1499999999999999</v>
+    <v>1.6189999999999998E-3</v>
+    <v>2.6290000000000003E-3</v>
+    <v>0.71</v>
     <v>USD</v>
-    <v>Adobe Inc is a United States-based global technology company. The Company's products, services and solutions are used around the world to imagine, create, manage, deliver, measure, optimize and engage with content across surfaces and fuel digital experiences. Its segments include digital media, digital experience, and publishing and advertising. The digital media segment is centered around Adobe Creative Cloud and Adobe Document Cloud, which include Adobe Express, Adobe Firefly, Photoshop and other products, offering a variety of tools for creative professionals, communicators and other consumers. The digital experience segment provides an integrated platform and set of products, services and solutions through Adobe Experience Cloud. The publishing and advertising segment contains legacy products and services. In addition, its Adobe GenStudio solution allows businesses to simplify their content supply chain process with generative artificial intelligence (AI) capabilities.</v>
-    <v>29945</v>
+    <v>Adobe Inc. is a global technology company. The Company's products, services and solutions are used around the world to imagine, create, manage, deliver, measure, optimize and engage with content across surfaces and fuel digital experiences. Its segments include Digital Media, Digital Experience, and Publishing and Advertising. The Digital Media segment is centered around Adobe Creative Cloud and Adobe Document Cloud, which include Adobe Express, Adobe Firefly, Photoshop and other products, offering a variety of tools for creative professionals, communicators and other consumers. The Digital Experience segment provides an integrated platform and set of products, services and solutions through Adobe Experience Cloud. The Publishing and Advertising segment contains legacy products and services. In addition, its Adobe GenStudio solution allows businesses to simplify their content supply chain process with generative artificial intelligence (AI) capabilities and intelligent automation.</v>
+    <v>30709</v>
     <v>Nasdaq Stock Market</v>
     <v>XNAS</v>
     <v>XNAS</v>
     <v>345 Park Avenue, SAN JOSE, CA, 95110-2704 US</v>
-    <v>422.66</v>
+    <v>442.74</v>
     <v>7</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45666.04159512656</v>
+    <v>45691.911737349219</v>
     <v>8</v>
-    <v>415.51</v>
-    <v>184699116000</v>
+    <v>430.88</v>
+    <v>190926571260</v>
     <v>ADOBE INC.</v>
     <v>ADOBE INC.</v>
-    <v>417.34</v>
-    <v>34.067999999999998</v>
-    <v>422.63</v>
-    <v>419.58</v>
-    <v>418.74</v>
-    <v>440200000</v>
+    <v>437.8</v>
+    <v>35.286999999999999</v>
+    <v>437.45</v>
+    <v>438.6</v>
+    <v>439.31</v>
+    <v>435309100</v>
     <v>ADBE</v>
     <v>ADOBE INC. (XNAS:ADBE)</v>
-    <v>3508786</v>
-    <v>4878015</v>
+    <v>3338798</v>
+    <v>3703753</v>
     <v>1997</v>
   </rv>
   <rv s="3">
@@ -2224,14 +2224,14 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>10</v>
-    <v>309.63</v>
+    <v>4</v>
+    <v>311.67129999999997</v>
     <v>231.27</v>
-    <v>0.80500000000000005</v>
-    <v>3.49</v>
-    <v>-6.5089999999999994E-4</v>
-    <v>1.2100999999999999E-2</v>
-    <v>-0.19</v>
+    <v>0.80589999999999995</v>
+    <v>4.3099999999999996</v>
+    <v>0</v>
+    <v>1.4224000000000001E-2</v>
+    <v>0</v>
     <v>USD</v>
     <v>Automatic Data Processing, Inc. (ADP) is a global technology company engaged in providing cloud-based human capital management (HCM) solutions that unite HR, payroll, talent, time, tax and benefits administration. Its segments include Employer Services and Professional Employer Organization (PEO). Its Employer Services segment serves clients ranging from single-employee small businesses to large enterprises with tens of thousands of employees around the world, offering a range of technology-based HCM solutions, including its cloud-based platforms, and human resource outsourcing (HRO) solutions (other than PEO) solutions. Its offerings include Payroll Services, Benefits Administration, Talent Management, HR Management, Workforce Management, Compliance Services, Insurance Services and Retirement Services. Its PEO business, called ADP TotalSource, provides clients with employment administration outsourcing solutions. ADP serves over 1.1 million clients in 140 countries and territories.</v>
     <v>64000</v>
@@ -2239,25 +2239,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>One Adp Boulvard, ROSELAND, NJ, 07068 US</v>
-    <v>292.05</v>
+    <v>307.94</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45665.995600798436</v>
+    <v>45691.910308066406</v>
     <v>11</v>
-    <v>288.51</v>
-    <v>118932594541</v>
+    <v>302.71499999999997</v>
+    <v>123286000000</v>
     <v>AUTOMATIC DATA PROCESSING, INC.</v>
     <v>AUTOMATIC DATA PROCESSING, INC.</v>
-    <v>288.51</v>
-    <v>31.1858</v>
-    <v>288.39999999999998</v>
-    <v>291.89</v>
-    <v>291.7</v>
-    <v>407456900</v>
+    <v>303.3</v>
+    <v>31.942</v>
+    <v>303.01</v>
+    <v>307.32</v>
+    <v>307.32</v>
+    <v>406870900</v>
     <v>ADP</v>
     <v>AUTOMATIC DATA PROCESSING, INC. (XNAS:ADP)</v>
-    <v>1513069</v>
-    <v>1805778</v>
+    <v>2168181</v>
+    <v>1629008</v>
     <v>1961</v>
   </rv>
   <rv s="3">
@@ -2278,14 +2278,14 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>10</v>
     <v>209.88</v>
-    <v>148.22999999999999</v>
-    <v>0.51900000000000002</v>
-    <v>5.76</v>
-    <v>-4.1710000000000002E-3</v>
-    <v>3.0960999999999999E-2</v>
-    <v>-0.8</v>
+    <v>153.87</v>
+    <v>0.51690000000000003</v>
+    <v>-0.35</v>
+    <v>0</v>
+    <v>-1.82E-3</v>
+    <v>0</v>
     <v>USD</v>
     <v>The Allstate Corporation is a holding company for Allstate Insurance Company. The Company's business is conducted principally through Allstate Insurance Company and other subsidiaries. It is primarily engaged in the property and casualty insurance business in the United States and Canada. It operates through five segments: Allstate Protection, Protection Services, Allstate Health and Benefits, Run-off Property-Liability, and Corporate &amp; Other. The Allstate Protection segment offers private passenger auto, homeowners, other personal lines, and commercial insurance through agents, contact centers and online. The Protection Services segment includes Allstate Protection Plans, Allstate Dealer Services, Allstate Roadside, Arity &amp; Allstate Identity Protection. The Allstate Health and Benefits segment offers voluntary benefits and individual life and health products, and other health insurance products. The Run-off Property-Liability segment includes property and casualty insurance coverage.</v>
     <v>53000</v>
@@ -2293,25 +2293,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>3100 SANDERS ROAD, NORTHBROOK, IL, 60062 US</v>
-    <v>191.84</v>
+    <v>192.77</v>
     <v>Insurance</v>
     <v>Stock</v>
-    <v>45666.035427117968</v>
+    <v>45691.888977939059</v>
     <v>14</v>
-    <v>185.02</v>
-    <v>50696620000</v>
+    <v>187.49</v>
+    <v>50836975930</v>
     <v>THE ALLSTATE CORPORATION</v>
     <v>THE ALLSTATE CORPORATION</v>
-    <v>188.72</v>
-    <v>12.3843</v>
-    <v>186.04</v>
-    <v>191.8</v>
-    <v>191</v>
+    <v>190.88</v>
+    <v>12.396000000000001</v>
+    <v>192.33</v>
+    <v>191.98</v>
+    <v>191.98</v>
     <v>264803500</v>
     <v>ALL</v>
     <v>THE ALLSTATE CORPORATION (XNYS:ALL)</v>
-    <v>2401720</v>
-    <v>1432072</v>
+    <v>1223713</v>
+    <v>1606765</v>
     <v>1992</v>
   </rv>
   <rv s="3">
@@ -2333,13 +2333,13 @@
     <v>3</v>
     <v>Finance</v>
     <v>4</v>
-    <v>233</v>
-    <v>146.15</v>
-    <v>1.1521999999999999</v>
-    <v>0.02</v>
-    <v>-3.2859999999999999E-3</v>
-    <v>9.0050000000000007E-5</v>
-    <v>-0.73</v>
+    <v>241.77</v>
+    <v>151.61000000000001</v>
+    <v>1.1567000000000001</v>
+    <v>-0.26</v>
+    <v>7.9179999999999997E-3</v>
+    <v>-1.0939999999999999E-3</v>
+    <v>1.88</v>
     <v>USD</v>
     <v>Amazon.com, Inc. provides a range of products and services to customers. The products offered through its stores include merchandise and content it has purchased for resale and products offered by third-party sellers. The Company’s segments include North America, International and Amazon Web Services (AWS). It serves consumers through its online and physical stores and focuses on selection, price, and convenience. Customers access its offerings through its Websites, mobile apps, Alexa, devices, streaming, and physically visiting its stores. It manufactures and sells electronic devices, including Kindle, Fire tablet, Fire TV, Echo, Ring, Blink, and eero, and it develops and produces media content. It serves developers and enterprises of all sizes, including start-ups, government agencies, and academic institutions, through AWS, which offers a broad set of on-demand technology services, including compute, storage, database, analytics, and machine learning, and other services.</v>
     <v>1551000</v>
@@ -2347,25 +2347,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>410 Terry Avenue North, SEATTLE, WA, 98109 US</v>
-    <v>223.52</v>
+    <v>239.25</v>
     <v>Diversified Retail</v>
     <v>Stock</v>
-    <v>45666.041660867966</v>
+    <v>45691.912201955471</v>
     <v>17</v>
-    <v>220.2</v>
-    <v>2335699171300</v>
+    <v>232.9</v>
+    <v>2496473674200</v>
     <v>AMAZON.COM, INC.</v>
     <v>AMAZON.COM, INC.</v>
-    <v>223.185</v>
-    <v>47.602600000000002</v>
-    <v>222.11</v>
-    <v>222.13</v>
-    <v>221.4</v>
+    <v>234.06</v>
+    <v>50.731900000000003</v>
+    <v>237.68</v>
+    <v>237.42</v>
+    <v>239.3</v>
     <v>10515010000</v>
     <v>AMZN</v>
     <v>AMAZON.COM, INC. (XNAS:AMZN)</v>
-    <v>25033292</v>
-    <v>35293001</v>
+    <v>37082906</v>
+    <v>30572765</v>
     <v>1996</v>
   </rv>
   <rv s="3">
@@ -2387,9 +2387,9 @@
     <v>12</v>
     <v>Finance</v>
     <v>13</v>
-    <v>0.88380000000000003</v>
-    <v>0.95</v>
-    <v>2.163E-3</v>
+    <v>0.8841</v>
+    <v>-2.85</v>
+    <v>-6.2909999999999997E-3</v>
     <v>EUR</v>
     <v>Berkshire Hathaway Inc. and its subsidiaries are engaged in diverse business activities, including insurance and reinsurance, utilities and energy, freight rail transportation, manufacturing, services and retailing. The Company’s segments include Insurance; Railroad (BNSF); Berkshire Hathaway Energy (BHE); Pilot Travel Centers (Pilot); Manufacturing; McLane Company (McLane), and Service and retailing. The Insurance segment includes GEICO, Berkshire Hathaway Primary Group and Berkshire Hathaway Reinsurance Group. The BNSF segment includes operation of railroad systems in North America through Burlington Northern Santa Fe, LLC. The BHE segment offers regulated electric and gas utilities. The Manufacturing segment manufacturers various products, including industrial, consumer and building products. The McLane segment is engaged in wholesale distribution of groceries and non-food items. The Pilot segment is an operator of travel centers in North America and a marketer of wholesale fuel.</v>
     <v>396500</v>
@@ -2397,24 +2397,24 @@
     <v>XWBO</v>
     <v>XWBO</v>
     <v>3555 Farnam Street, OMAHA, NE, 68131 US</v>
-    <v>440.7</v>
+    <v>453.5</v>
     <v>Consumer Goods Conglomerates</v>
     <v>Stock</v>
-    <v>45665</v>
+    <v>45691</v>
     <v>20</v>
-    <v>437.85</v>
-    <v>978680400000</v>
+    <v>448.4</v>
+    <v>1010430000000</v>
     <v>BERKSHIRE HATHAWAY INC.</v>
     <v>BERKSHIRE HATHAWAY INC.</v>
-    <v>438.9</v>
-    <v>9.8800000000000008</v>
-    <v>439.2</v>
-    <v>440.15</v>
+    <v>452.5</v>
+    <v>10.1248</v>
+    <v>453</v>
+    <v>450.15</v>
     <v>1437610</v>
     <v>BRKB</v>
     <v>BERKSHIRE HATHAWAY INC. (XWBO:BRKB)</v>
-    <v>47</v>
-    <v>1400</v>
+    <v>101</v>
+    <v>1580</v>
     <v>1998</v>
   </rv>
   <rv s="3">
@@ -2437,12 +2437,12 @@
     <v>Finance</v>
     <v>4</v>
     <v>418.5</v>
-    <v>276.94</v>
-    <v>1.1082000000000001</v>
-    <v>-1.93</v>
-    <v>-1.163E-3</v>
-    <v>-5.3169999999999997E-3</v>
-    <v>-0.42</v>
+    <v>307.05</v>
+    <v>1.1067</v>
+    <v>-9.93</v>
+    <v>7.1909999999999995E-3</v>
+    <v>-2.6734000000000001E-2</v>
+    <v>2.6</v>
     <v>USD</v>
     <v>Caterpillar Inc. is a manufacturer of construction and mining equipment, off-highway diesel and natural gas engines, industrial gas turbines and diesel-electric locomotives. The Company operates through its three primary segments: Construction Industries, Resource Industries and Energy &amp; Transportation. It also provides financing and related services through its Financial Products segment. The Construction Industries segment is primarily responsible for supporting customers using machinery in infrastructure and building construction applications. The Resource Industries segment is primarily responsible for supporting customers using machinery in mining, heavy construction and quarry and aggregates. The Energy &amp; Transportation segment is primarily responsible for supporting customers using reciprocating engines, turbines, diesel-electric locomotives, and related services across industries serving oil and gas, power generation, industrial and transportation applications.</v>
     <v>113200</v>
@@ -2450,25 +2450,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>5205 N. O'connor Boulevard, Suite 100, IRVING, TX, 75039 US</v>
-    <v>362.88</v>
+    <v>368.55</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45666.031677117971</v>
+    <v>45691.911315092184</v>
     <v>23</v>
-    <v>357.7</v>
-    <v>175638700000</v>
+    <v>359.69</v>
+    <v>174537931775</v>
     <v>CATERPILLAR INC.</v>
     <v>CATERPILLAR INC.</v>
-    <v>362.45</v>
-    <v>16.7454</v>
-    <v>363</v>
-    <v>361.07</v>
-    <v>360.65</v>
+    <v>364.14</v>
+    <v>16.3797</v>
+    <v>371.44</v>
+    <v>361.51</v>
+    <v>364.15</v>
     <v>482802500</v>
     <v>CAT</v>
     <v>CATERPILLAR INC. (XNYS:CAT)</v>
-    <v>1828830</v>
-    <v>1784606</v>
+    <v>3072855</v>
+    <v>2105937</v>
     <v>1986</v>
   </rv>
   <rv s="3">
@@ -2490,13 +2490,13 @@
     <v>3</v>
     <v>Finance</v>
     <v>4</v>
-    <v>1008.25</v>
-    <v>654.03380000000004</v>
-    <v>0.83650000000000002</v>
-    <v>6</v>
-    <v>1.8794999999999999E-2</v>
-    <v>6.5120000000000004E-3</v>
-    <v>17.43</v>
+    <v>1009.6105</v>
+    <v>697.27</v>
+    <v>0.8397</v>
+    <v>25.95</v>
+    <v>1.114E-3</v>
+    <v>2.6483E-2</v>
+    <v>1.1200000000000001</v>
     <v>USD</v>
     <v>Costco Wholesale Corporation (Costco) operates membership warehouses and e-commerce sites that offer a selection of nationally branded and private-label products in a wide range of categories. The Company buys the majority of its merchandise directly from suppliers and route it to cross-docking consolidation points (depots) or directly to its warehouses. It operates 891 warehouses, including 614 in the United States and Puerto Rico, 108 in Canada, 40 in Mexico, 35 in Japan, 29 in the United Kingdom, 19 in Korea, 15 in Australia, 14 in Taiwan, seven in China, five in Spain, two in France, and one each in Iceland, New Zealand and Sweden. It also operates e-commerce sites in the United States, Canada, the United Kingdom, Mexico, Korea, Taiwan, Japan and Australia. The Company provides wide selection of merchandise, plus the convenience of specialty departments and exclusive member services.</v>
     <v>333000</v>
@@ -2504,25 +2504,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>999 Lake Dr, ISSAQUAH, WA, 98027- US</v>
-    <v>930.49990000000003</v>
+    <v>1009.6105</v>
     <v>Diversified Retail</v>
     <v>Stock</v>
-    <v>45666.04159179375</v>
+    <v>45691.912147256247</v>
     <v>26</v>
-    <v>915.41499999999996</v>
-    <v>411658522893</v>
+    <v>968.94</v>
+    <v>446486830587</v>
     <v>COSTCO WHOLESALE CORPORATION</v>
     <v>COSTCO WHOLESALE CORPORATION</v>
-    <v>922.97500000000002</v>
-    <v>54.103099999999998</v>
-    <v>921.37</v>
-    <v>927.37</v>
-    <v>944.8</v>
+    <v>972.38499999999999</v>
+    <v>57.538800000000002</v>
+    <v>979.88</v>
+    <v>1005.83</v>
+    <v>1006.95</v>
     <v>443898900</v>
     <v>COST</v>
     <v>COSTCO WHOLESALE CORPORATION (XNAS:COST)</v>
-    <v>1774763</v>
-    <v>2069934</v>
+    <v>2666385</v>
+    <v>1836131</v>
     <v>1987</v>
   </rv>
   <rv s="3">
@@ -2595,12 +2595,12 @@
     <v>Finance</v>
     <v>4</v>
     <v>168.07</v>
-    <v>70.150000000000006</v>
-    <v>0.43819999999999998</v>
-    <v>-2.5499999999999998</v>
-    <v>2.513E-3</v>
-    <v>-3.4380000000000001E-2</v>
-    <v>0.18</v>
+    <v>66.430000000000007</v>
+    <v>0.43240000000000001</v>
+    <v>0.41</v>
+    <v>5.457E-3</v>
+    <v>5.77E-3</v>
+    <v>0.39</v>
     <v>USD</v>
     <v>Dollar General Corporation is a discount retailer. The Company offers merchandise, including consumable items, seasonal items, home products and apparel. Its merchandise includes brands from manufacturers, as well as its own private brand selections with prices at discounts to brands. Its consumables category includes paper and cleaning products, packaged food, perishables, snacks, health and beauty, pet, and tobacco products. Its seasonal products include holiday items, toys, batteries, small electronics, greeting cards, stationery, prepaid phones and accessories, gardening supplies, hardware, automotive and home office supplies. Its home products include kitchen supplies, cookware, small appliances, light bulbs, storage containers, frames, candles, craft supplies and kitchen, bed and bath soft goods. The Company’s apparel products include basic items for infants, toddlers, girls, boys, women and men, as well as socks, underwear, disposable diapers, shoes and accessories.</v>
     <v>185800</v>
@@ -2608,25 +2608,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>100 Mission Ridge, GOODLETTSVILLE, TN, 37072-2171 US</v>
-    <v>74</v>
+    <v>72.69</v>
     <v>Diversified Retail</v>
     <v>Stock</v>
-    <v>45666.040316099221</v>
+    <v>45691.909786191405</v>
     <v>32</v>
-    <v>70.150000000000006</v>
-    <v>16421850000</v>
+    <v>69.319999999999993</v>
+    <v>15718089779</v>
     <v>DOLLAR GENERAL CORPORATION</v>
     <v>DOLLAR GENERAL CORPORATION</v>
-    <v>73.790000000000006</v>
-    <v>11.7949</v>
-    <v>74.17</v>
-    <v>71.62</v>
-    <v>71.8</v>
+    <v>70.09</v>
+    <v>11.770200000000001</v>
+    <v>71.06</v>
+    <v>71.47</v>
+    <v>71.86</v>
     <v>219925700</v>
     <v>DG</v>
     <v>DOLLAR GENERAL CORPORATION (XNYS:DG)</v>
-    <v>5786143</v>
-    <v>4089958</v>
+    <v>3847297</v>
+    <v>3464970</v>
     <v>1998</v>
   </rv>
   <rv s="3">
@@ -2649,12 +2649,12 @@
     <v>Finance</v>
     <v>4</v>
     <v>281.7</v>
-    <v>222.53</v>
-    <v>0.84099999999999997</v>
-    <v>-1.01</v>
-    <v>-3.5279999999999999E-3</v>
-    <v>-4.2240000000000003E-3</v>
-    <v>-0.84</v>
+    <v>214.03</v>
+    <v>0.83609999999999995</v>
+    <v>-8.5399999999999991</v>
+    <v>1.1200000000000001E-3</v>
+    <v>-3.8341E-2</v>
+    <v>0.24</v>
     <v>USD</v>
     <v>Danaher Corporation is a global life sciences and diagnostics innovator. The Company operates through three business segments: Biotechnology, Life Sciences and Diagnostics. The Biotechnology segment includes the bioprocessing and discovery and medical businesses and offers a broad range of equipment, consumables and services that are primarily used by customers to advance and accelerate the research, development, manufacture and delivery of biological medicines. The Life Sciences segment offers a range of instruments, consumables, services and software that are primarily used by customers to study genomics and the basic building blocks of life, including deoxyribonucleic acid (DNA)and ribonucleic acid (RNA), nucleic acid, proteins, metabolites and cells. The Diagnostics segment offers clinical instruments, consumables, software and services that hospitals, physicians’ offices, reference laboratories and other critical care settings use to diagnose disease and make treatment decisions.</v>
     <v>61000</v>
@@ -2662,25 +2662,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>2200 Pennsylvania Ave NW Ste 800W, WASHINGTON, DC, 20037-1701 US</v>
-    <v>239.39</v>
+    <v>219.94</v>
     <v>Healthcare Equipment &amp; Supplies</v>
     <v>Stock</v>
-    <v>45666.017824293747</v>
+    <v>45691.91172579844</v>
     <v>35</v>
-    <v>235.5</v>
-    <v>169619100000</v>
+    <v>214.03</v>
+    <v>154031220000</v>
     <v>DANAHER CORPORATION</v>
     <v>DANAHER CORPORATION</v>
-    <v>238.61</v>
-    <v>44.945500000000003</v>
-    <v>239.1</v>
-    <v>238.09</v>
-    <v>237.25</v>
-    <v>722275100</v>
+    <v>218</v>
+    <v>40.520600000000002</v>
+    <v>222.74</v>
+    <v>214.2</v>
+    <v>214.5</v>
+    <v>719100000</v>
     <v>DHR</v>
     <v>DANAHER CORPORATION (XNYS:DHR)</v>
-    <v>2527729</v>
-    <v>3247194</v>
+    <v>5785465</v>
+    <v>3296176</v>
     <v>1986</v>
   </rv>
   <rv s="3">
@@ -2720,38 +2720,38 @@
     <v>4</v>
     <v>123.74</v>
     <v>83.91</v>
-    <v>1.4280999999999999</v>
-    <v>-1.63</v>
-    <v>1.2025999999999998E-2</v>
-    <v>-1.4633E-2</v>
-    <v>1.32</v>
+    <v>1.4273</v>
+    <v>1</v>
+    <v>3.5530000000000002E-3</v>
+    <v>8.8449999999999987E-3</v>
+    <v>0.40500000000000003</v>
     <v>USD</v>
-    <v>The Walt Disney Company is a diversified worldwide entertainment company. The Company's segments include Entertainment, Sports and Experiences. The Entertainment segment generally encompasses the Company’s non-sports focused global film, television and direct-to-consumer (DTC) video streaming content production and distribution activities. Its line of business includes Linear Networks, Direct-to-Consumer, and Content Sales/Licensing. The Sports segment generally encompasses the Company’s sports-focused global television and DTC video streaming content production and distribution activities. Its line of business includes ESPN and Star. Experiences segment includes Parks and Experiences and Consumer Products. Parks and Experiences consists of Walt Disney World Resort in Florida, Disneyland Resort in California, Disney Cruise Line, Disney Vacation Club, and Disneyland Paris, among others. Consumer Products includes licensing of its trade names, characters, visual, literary and other IPs.</v>
+    <v>The Walt Disney Company is a diversified worldwide entertainment company. The Company's segments include Entertainment, Sports and Experiences. The Entertainment segment generally encompasses its non-sports focused global film and episodic content production and distribution activities. The lines of business within the Entertainment segment along with their business activities include Linear Networks, Direct-to-Consumer, and Content Sales/Licensing. The Sports segment encompasses its sports-focused global television and direct-to-consumer (DTC) video streaming content production and distribution activities. The lines of business within the Sports segment include ESPN and Star. The Experiences segment includes Parks and Experiences and Consumer Products. Parks and Experiences consists of Walt Disney World Resort in Florida, Disneyland Resort in California, Disney Cruise Line, and others. Consumer Products includes licensing of its trade names, characters, visual, literary and other IP.</v>
     <v>233000</v>
     <v>New York Stock Exchange</v>
     <v>XNYS</v>
     <v>XNYS</v>
     <v>500 South Buena Vista Street, BURBANK, CA, 91521-0001 US</v>
-    <v>111.11</v>
+    <v>114.6</v>
     <v>40</v>
     <v>Media &amp; Publishing</v>
     <v>Stock</v>
-    <v>45666.041522742969</v>
+    <v>45691.912151423436</v>
     <v>41</v>
-    <v>108.64</v>
-    <v>201304000000</v>
+    <v>110.86</v>
+    <v>206272947600</v>
     <v>THE WALT DISNEY COMPANY</v>
     <v>THE WALT DISNEY COMPANY</v>
-    <v>111</v>
-    <v>40.406399999999998</v>
-    <v>111.39</v>
-    <v>109.76</v>
-    <v>111.08</v>
-    <v>1810939000</v>
+    <v>111.35</v>
+    <v>41.989400000000003</v>
+    <v>113.06</v>
+    <v>114.06</v>
+    <v>114.405</v>
+    <v>1808460000</v>
     <v>DIS</v>
     <v>THE WALT DISNEY COMPANY (XNYS:DIS)</v>
-    <v>7805312</v>
-    <v>7714529</v>
+    <v>8852592</v>
+    <v>6772419</v>
     <v>2018</v>
   </rv>
   <rv s="3">
@@ -2773,13 +2773,13 @@
     <v>3</v>
     <v>Finance</v>
     <v>4</v>
-    <v>202.88</v>
+    <v>207.08</v>
     <v>131.55000000000001</v>
-    <v>0.9869</v>
-    <v>-1.32</v>
-    <v>-1.9959999999999999E-3</v>
-    <v>-6.7100000000000007E-3</v>
-    <v>-0.39</v>
+    <v>0.99099999999999999</v>
+    <v>-2.96</v>
+    <v>7.6E-3</v>
+    <v>-1.4397E-2</v>
+    <v>1.54</v>
     <v>USD</v>
     <v>Alphabet Inc. is a holding company. The Company's segments include Google Services, Google Cloud, and Other Bets. The Google Services segment includes products and services such as ads, Android, Chrome, devices, Google Maps, Google Play, Search, and YouTube. The Google Cloud segment includes infrastructure and platform services, collaboration tools, and other services for enterprise customers. Its Other Bets segment is engaged in the sale of healthcare-related services and Internet services. Its Google Cloud provides enterprise-ready cloud services, including Google Cloud Platform and Google Workspace. Google Cloud Platform provides access to solutions such as cybersecurity, databases, analytics, and artificial intelligence (AI) offerings, including its AI infrastructure, Vertex AI platform, and Duet AI for Google Cloud. Google Workspace includes cloud-based communication and collaboration tools for enterprises, such as Calendar, Gmail, Docs, Drive, Meet and other enterprise services.</v>
     <v>181269</v>
@@ -2787,25 +2787,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>1600 Amphitheatre Parkway, MOUNTAIN VIEW, CA, 94043 US</v>
-    <v>197.64</v>
+    <v>205.22</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45666.04136091406</v>
+    <v>45691.912173853903</v>
     <v>44</v>
-    <v>193.75</v>
-    <v>2399745000000</v>
+    <v>201.66</v>
+    <v>2506153000000</v>
     <v>ALPHABET INC.</v>
     <v>ALPHABET INC.</v>
-    <v>193.95</v>
-    <v>26.080500000000001</v>
-    <v>196.71</v>
-    <v>195.39</v>
-    <v>195</v>
+    <v>202.215</v>
+    <v>26.866800000000001</v>
+    <v>205.6</v>
+    <v>202.64</v>
+    <v>204.18</v>
     <v>12241000000</v>
     <v>GOOG</v>
     <v>ALPHABET INC. (XNAS:GOOG)</v>
-    <v>14335341</v>
-    <v>20575204</v>
+    <v>16561462</v>
+    <v>15218438</v>
     <v>2015</v>
   </rv>
   <rv s="3">
@@ -2829,11 +2829,11 @@
     <v>4</v>
     <v>439.37</v>
     <v>323.77</v>
-    <v>1.0556000000000001</v>
-    <v>2.97</v>
-    <v>-2.0660000000000001E-3</v>
-    <v>7.7299999999999999E-3</v>
-    <v>-0.8</v>
+    <v>1.0584</v>
+    <v>-3.16</v>
+    <v>7.8040000000000002E-3</v>
+    <v>-7.6699999999999997E-3</v>
+    <v>3.19</v>
     <v>USD</v>
     <v>The Home Depot, Inc. is a home improvement retailer. The Company offers a wide assortment of building materials, home improvement products, lawn and garden products, decor products, and facilities maintenance, repair, and operations products. It also provides various services, including home improvement installation services and tool and equipment rental. The Company operates approximately 2,335 stores located throughout the United States including the Commonwealth of Puerto Rico and the territories of the U.S. Virgin Islands and Guam, Canada, and Mexico. The Home Depot stores average approximately 104,000 square feet of enclosed space, with approximately 24,000 additional square feet of outside garden area. It also maintains a network of distribution and fulfillment centers, as well as various e-commerce websites in the United States, Canada, and Mexico. The Company serves two primary customer groups: do-it-yourself (DIY) Customers and Professional Customers (Pros).</v>
     <v>463100</v>
@@ -2841,25 +2841,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>2455 Paces Ferry Road, ATLANTA, GA, 30339 US</v>
-    <v>387.69</v>
+    <v>411.9</v>
     <v>Specialty Retailers</v>
     <v>Stock</v>
-    <v>45666.037176527345</v>
+    <v>45691.911177765622</v>
     <v>47</v>
-    <v>380.1</v>
-    <v>386596900000</v>
+    <v>401.01</v>
+    <v>406106498132</v>
     <v>THE HOME DEPOT, INC.</v>
     <v>THE HOME DEPOT, INC.</v>
-    <v>383</v>
-    <v>26.302</v>
-    <v>384.23</v>
-    <v>387.2</v>
-    <v>386.4</v>
+    <v>406.12</v>
+    <v>27.770600000000002</v>
+    <v>411.98</v>
+    <v>408.82</v>
+    <v>411.95</v>
     <v>993362600</v>
     <v>HD</v>
     <v>THE HOME DEPOT, INC. (XNYS:HD)</v>
-    <v>2848462</v>
-    <v>3026808</v>
+    <v>2895326</v>
+    <v>2911857</v>
     <v>1978</v>
   </rv>
   <rv s="3">
@@ -2882,12 +2882,12 @@
     <v>Finance</v>
     <v>4</v>
     <v>242.77</v>
-    <v>189.66</v>
-    <v>1.0485</v>
-    <v>-0.46</v>
-    <v>-9.992E-4</v>
-    <v>-2.085E-3</v>
-    <v>-0.22</v>
+    <v>189.75</v>
+    <v>1.0452999999999999</v>
+    <v>-1.31</v>
+    <v>0</v>
+    <v>-5.8560000000000001E-3</v>
+    <v>0</v>
     <v>USD</v>
     <v>Honeywell International Inc. is an integrated operating company. Its Aerospace Technologies segment supplies products, software, and services for aircraft that it sells to original equipment manufacturers and other customers in a variety of end markets, including air transport, regional, business and general aviation aircraft, airlines, aircraft operators, and others. Its Industrial Automation segment provides industrial automation solutions that deliver intelligent, sustainable, and secure operations for customers in oil and gas, petrochemicals, life sciences, metals and mining, and other segments. The Energy and Sustainability Solutions segment consists of UOP, advanced materials business units and LNG process technology and equipment business. The Building Automation segment offers products, software, security access solutions, and technologies that enable building owners and occupants to ensure their facilities are safe, energy efficient, sustainable, and productive.</v>
     <v>95000</v>
@@ -2895,25 +2895,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>855 S. Mint Street, CHARLOTTE, NC, 28202 US</v>
-    <v>221.38</v>
+    <v>223.3</v>
     <v>Consumer Goods Conglomerates</v>
     <v>Stock</v>
-    <v>45666.040090034374</v>
+    <v>45691.910308089842</v>
     <v>50</v>
-    <v>219.2</v>
-    <v>143164970058</v>
+    <v>219.66329999999999</v>
+    <v>144621524234</v>
     <v>HONEYWELL INTERNATIONAL INCORPORATION</v>
     <v>HONEYWELL INTERNATIONAL INCORPORATION</v>
-    <v>220.09</v>
-    <v>25.484300000000001</v>
-    <v>220.63</v>
-    <v>220.17</v>
-    <v>219.95</v>
+    <v>222.5</v>
+    <v>25.675999999999998</v>
+    <v>223.72</v>
+    <v>222.41</v>
+    <v>222.41</v>
     <v>650247400</v>
     <v>HON</v>
     <v>HONEYWELL INTERNATIONAL INCORPORATION (XNAS:HON)</v>
-    <v>3120530</v>
-    <v>3718038</v>
+    <v>3215204</v>
+    <v>3301231</v>
     <v>1985</v>
   </rv>
   <rv s="3">
@@ -2936,12 +2936,12 @@
     <v>Finance</v>
     <v>4</v>
     <v>168.85</v>
-    <v>141.44</v>
-    <v>0.50700000000000001</v>
-    <v>-3.96</v>
-    <v>-1.406E-4</v>
-    <v>-2.7081000000000001E-2</v>
-    <v>-0.02</v>
+    <v>140.68</v>
+    <v>0.5111</v>
+    <v>-0.28000000000000003</v>
+    <v>2.0409999999999998E-3</v>
+    <v>-1.8400000000000001E-3</v>
+    <v>0.31</v>
     <v>USD</v>
     <v>Johnson &amp; Johnson, through its subsidiaries, is engaged in the research and development, manufacture, and sale of a range of products in the healthcare field. The Company's primary focus is products related to human health and well-being. It operates through two segments: Innovative Medicine and MedTech. The Innovative Medicine segment is focused on various therapeutic areas, including immunology, infectious diseases, neuroscience, oncology, pulmonary hypertension, and cardiovascular and metabolic diseases. Products in this segment are distributed directly to retailers, wholesalers, distributors, hospitals, and healthcare professionals for prescription use. The MedTech segment includes a broad portfolio of products used in the orthopedic, surgery, interventional solutions, cardiovascular intervention, and vision fields. The MedTech segment also offers a commercially available intravascular lithotripsy (IVL) platform for coronary artery disease (CAD) and peripheral artery disease (PAD).</v>
     <v>131900</v>
@@ -2949,25 +2949,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>One Johnson &amp; Johnson Plaza, NEW BRUNSWICK, NJ, 08933 US</v>
-    <v>145.59</v>
+    <v>152.465</v>
     <v>Pharmaceuticals</v>
     <v>Stock</v>
-    <v>45666.041326978906</v>
+    <v>45691.912111307814</v>
     <v>53</v>
-    <v>141.44</v>
-    <v>347155200000</v>
+    <v>150.78</v>
+    <v>365645705010</v>
     <v>JOHNSON &amp; JOHNSON</v>
     <v>JOHNSON &amp; JOHNSON</v>
-    <v>145.49</v>
-    <v>23.3874</v>
-    <v>146.22999999999999</v>
-    <v>142.27000000000001</v>
-    <v>142.25</v>
+    <v>152</v>
+    <v>26.196200000000001</v>
+    <v>152.15</v>
+    <v>151.87</v>
+    <v>152.18</v>
     <v>2407623000</v>
     <v>JNJ</v>
     <v>JOHNSON &amp; JOHNSON (XNYS:JNJ)</v>
-    <v>11175552</v>
-    <v>8244132</v>
+    <v>6679846</v>
+    <v>8732781</v>
     <v>1887</v>
   </rv>
   <rv s="3">
@@ -2991,37 +2991,37 @@
     <v>4</v>
     <v>618.95000000000005</v>
     <v>413.92</v>
-    <v>0.4879</v>
-    <v>4.8899999999999997</v>
-    <v>-2.5590000000000004E-4</v>
-    <v>1.0540000000000001E-2</v>
-    <v>-0.12</v>
+    <v>0.48230000000000001</v>
+    <v>-7.55</v>
+    <v>5.006E-3</v>
+    <v>-1.6308E-2</v>
+    <v>2.2799999999999998</v>
     <v>USD</v>
-    <v>Lockheed Martin Corporation is a global security and aerospace company. The Company is engaged in the research, design, development, manufacture, integration and sustainment of advanced technology systems, products and services. Its segments include Aeronautics, Missiles and Fire Control (MFC), Rotary and Mission Systems (RMS) and Space. Aeronautics segment is engaged in the research, design, development, manufacture, integration, sustainment, support and upgrade of advanced military aircraft. MFC segment provides air and missile defense systems, manned and unmanned ground vehicles, energy management solutions, and others. RMS segment designs, manufactures, services and supports various military and commercial helicopters, surface ships, sea and land-based missile defense systems, and others. Space segment is engaged in the research and design, development, engineering and production of satellites, space transportation systems, and strategic, advanced strike, and defensive systems.</v>
-    <v>122000</v>
+    <v>Lockheed Martin Corporation is a global aerospace and defense company. The Company is engaged in the research, design, development, manufacture, integration and sustainment of advanced technology systems, products and services. Its segments include Aeronautics, Missiles and Fire Control (MFC), Rotary and Mission Systems (RMS) and Space. Aeronautics segment is engaged in the research, design, development, manufacture, integration, sustainment, support and upgrade of advanced military aircraft. MFC segment provides air and missile defense systems, manned and unmanned ground vehicles, energy management solutions, and others. RMS segment designs, manufactures, services and supports various military and commercial helicopters, surface ships, sea and land-based missile defense systems, and others. Its Space segment is engaged in the research and design, development, engineering and production of satellites, space transportation systems, and strategic, advanced strike, and defensive systems.</v>
+    <v>121000</v>
     <v>New York Stock Exchange</v>
     <v>XNYS</v>
     <v>XNYS</v>
     <v>6801 ROCKLEDGE DR, BETHESDA, MD, 20817 US</v>
-    <v>469.22</v>
+    <v>461.33199999999999</v>
     <v>Aerospace &amp; Defense</v>
     <v>Stock</v>
-    <v>45666.036400693753</v>
+    <v>45691.909656527343</v>
     <v>56</v>
-    <v>461.24</v>
-    <v>114208300000</v>
+    <v>453.57499999999999</v>
+    <v>107194738860</v>
     <v>LOCKHEED MARTIN CORPORATION</v>
     <v>LOCKHEED MARTIN CORPORATION</v>
-    <v>463.5</v>
-    <v>16.958600000000001</v>
-    <v>463.96</v>
-    <v>468.85</v>
-    <v>468.73</v>
-    <v>237035300</v>
+    <v>458.8</v>
+    <v>20.450199999999999</v>
+    <v>462.95</v>
+    <v>455.4</v>
+    <v>457.7</v>
+    <v>235385900</v>
     <v>LMT</v>
     <v>LOCKHEED MARTIN CORPORATION (XNYS:LMT)</v>
-    <v>998673</v>
-    <v>1260931</v>
+    <v>1475001</v>
+    <v>1299826</v>
     <v>1994</v>
   </rv>
   <rv s="3">
@@ -3043,13 +3043,13 @@
     <v>3</v>
     <v>Finance</v>
     <v>4</v>
-    <v>537.70000000000005</v>
-    <v>416.53</v>
-    <v>1.101</v>
-    <v>5</v>
-    <v>-7.7459999999999996E-4</v>
-    <v>9.777000000000001E-3</v>
-    <v>-0.4</v>
+    <v>576.94000000000005</v>
+    <v>428.86</v>
+    <v>1.1032</v>
+    <v>8.9109999999999996</v>
+    <v>4.522E-3</v>
+    <v>1.6043000000000002E-2</v>
+    <v>2.5499999999999998</v>
     <v>USD</v>
     <v>Mastercard Incorporated is a technology company that connects consumers, financial institutions, merchants, governments and businesses across the world, enabling them to use electronic forms of payment. It allows users to make payments by creating a range of payment solutions and services using its brands: MasterCard, Maestro and Cirrus. It enables a variety of payments capabilities (including products and value-added services and solutions) over its multi-rail network among account holders, merchants, financial institutions, businesses, governments and others, offering customers one partner for their payment needs. Its products include consumer credit, consumer debit, prepaid, B2B accounts payable, commercial point of sale, disbursements and remittances, and others. It offers additional payment capabilities that include automated clearing house (ACH) transactions (both batch and real-time account-based payments). It also offers other services, such as cyber and intelligence solutions.</v>
     <v>33400</v>
@@ -3057,25 +3057,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>2000 Purchase St, PURCHASE, NY, 10577 US</v>
-    <v>517.45000000000005</v>
+    <v>565</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45666.02499008047</v>
+    <v>45691.910338923437</v>
     <v>59</v>
-    <v>511.53250000000003</v>
-    <v>478520400000</v>
+    <v>551.07000000000005</v>
+    <v>515807674000</v>
     <v>MASTERCARD INCORPORATED.</v>
     <v>MASTERCARD INCORPORATED.</v>
-    <v>512.04</v>
-    <v>39.033099999999997</v>
-    <v>511.4</v>
-    <v>516.4</v>
-    <v>516</v>
-    <v>917831100</v>
+    <v>552.64</v>
+    <v>40.626100000000001</v>
+    <v>555.42999999999995</v>
+    <v>564.34100000000001</v>
+    <v>566.5</v>
+    <v>914000000</v>
     <v>MA</v>
     <v>MASTERCARD INCORPORATED. (XNYS:MA)</v>
-    <v>2456715</v>
-    <v>2504001</v>
+    <v>3195095</v>
+    <v>2601804</v>
     <v>2001</v>
   </rv>
   <rv s="3">
@@ -3114,12 +3114,12 @@
     <v>Finance</v>
     <v>4</v>
     <v>468.35</v>
-    <v>369.01</v>
-    <v>0.89910000000000001</v>
-    <v>2.19</v>
-    <v>-2.2729999999999998E-3</v>
-    <v>5.1849999999999995E-3</v>
-    <v>-0.96499999999999997</v>
+    <v>385.58</v>
+    <v>0.89470000000000005</v>
+    <v>-4.1399999999999997</v>
+    <v>5.1830000000000001E-3</v>
+    <v>-9.9740000000000002E-3</v>
+    <v>2.13</v>
     <v>USD</v>
     <v>Microsoft Corporation is a technology company. The Company develops and supports software, services, devices, and solutions. The Company’s segments include Productivity and Business Processes, Intelligent Cloud, and More Personal Computing. The Productivity and Business Processes segment consists of products and services in its portfolio of productivity, communication, and information services. This segment primarily comprises: Office Commercial, Office Consumer, LinkedIn, and Dynamics business solutions. The Intelligent Cloud segment consists of server products and cloud services, including Azure and other cloud services, SQL Server, Windows Server, Visual Studio, System Center, and related Client Access Licenses (CALs), and Nuance and GitHub; and Enterprise Services, including enterprise support services, industry solutions and Nuance professional services. The More Personal Computing segment primarily comprises Windows, Devices, Gaming, and search and news advertising.</v>
     <v>228000</v>
@@ -3127,26 +3127,26 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>One Microsoft Way, REDMOND, WA, 98052-6399 US</v>
-    <v>426.97</v>
+    <v>415.41</v>
     <v>64</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45666.041650682811</v>
+    <v>45691.912226330467</v>
     <v>65</v>
-    <v>421.54</v>
-    <v>3156553077360</v>
+    <v>408.66</v>
+    <v>3054771883440</v>
     <v>MICROSOFT CORPORATION</v>
     <v>MICROSOFT CORPORATION</v>
-    <v>423.46</v>
-    <v>34.933300000000003</v>
-    <v>422.37</v>
-    <v>424.56</v>
-    <v>423.59500000000003</v>
-    <v>7434881000</v>
+    <v>411.6</v>
+    <v>33.100299999999997</v>
+    <v>415.06</v>
+    <v>410.92</v>
+    <v>413.05</v>
+    <v>7433982000</v>
     <v>MSFT</v>
     <v>MICROSOFT CORPORATION (XNAS:MSFT)</v>
-    <v>15054575</v>
-    <v>20487215</v>
+    <v>25502440</v>
+    <v>20898000</v>
     <v>1993</v>
   </rv>
   <rv s="3">
@@ -3170,11 +3170,11 @@
     <v>4</v>
     <v>86.1</v>
     <v>53.95</v>
-    <v>0.57820000000000005</v>
-    <v>0.23</v>
-    <v>-1.132E-3</v>
-    <v>3.2659999999999998E-3</v>
-    <v>-0.08</v>
+    <v>0.57679999999999998</v>
+    <v>-0.49</v>
+    <v>4.7850000000000002E-3</v>
+    <v>-6.8469999999999998E-3</v>
+    <v>0.34</v>
     <v>USD</v>
     <v>NextEra Energy, Inc. is an electric power and energy infrastructure company. It operates through its wholly owned subsidiaries, NextEra Energy Resources, LLC and NextEra Energy Transmission, LLC (collectively, NEER) and Florida Power &amp; Light Company (FPL). Its segments include NEER and FPL. FPL segment is a rate-regulated electric utility engaged in the generation, transmission, distribution and sale of electric energy in Florida. FPL has approximately 33,276 megawatts (MW) of net generating capacity, approximately 90,000 circuit miles of transmission and distribution lines and 883 substations. The NEER segment owns, develops, constructs, manages and operates electric generation facilities in wholesale energy markets in the United States and Canada and also includes assets and investments in other businesses with a clean energy focus, such as battery storage and renewable fuels. It also owns, develops, constructs and operates rate-regulated transmission facilities in North America.</v>
     <v>16800</v>
@@ -3182,25 +3182,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>700 Universe Blvd, JUNO BEACH, FL, 33408 US</v>
-    <v>70.7</v>
+    <v>71.790000000000006</v>
     <v>Electrical Utilities &amp; IPPs</v>
     <v>Stock</v>
-    <v>45666.037793274998</v>
+    <v>45691.911148807812</v>
     <v>68</v>
-    <v>69.459999999999994</v>
-    <v>148040600000</v>
+    <v>70.19</v>
+    <v>146148703350</v>
     <v>NEXTERA ENERGY, INC.</v>
     <v>NEXTERA ENERGY, INC.</v>
-    <v>70.02</v>
-    <v>20.956199999999999</v>
-    <v>70.430000000000007</v>
-    <v>70.66</v>
-    <v>70.58</v>
+    <v>70.5</v>
+    <v>21.0671</v>
+    <v>71.56</v>
+    <v>71.069999999999993</v>
+    <v>71.39</v>
     <v>2056405000</v>
     <v>NEE</v>
     <v>NEXTERA ENERGY, INC. (XNYS:NEE)</v>
-    <v>7930615</v>
-    <v>8633617</v>
+    <v>9127890</v>
+    <v>10762291</v>
     <v>1984</v>
   </rv>
   <rv s="3">
@@ -3222,9 +3222,9 @@
     <v>17</v>
     <v>Finance</v>
     <v>13</v>
-    <v>1.0154000000000001</v>
-    <v>-0.65</v>
-    <v>-9.3139999999999994E-3</v>
+    <v>1.0152000000000001</v>
+    <v>-0.57999999999999996</v>
+    <v>-7.7449999999999993E-3</v>
     <v>EUR</v>
     <v>NIKE, Inc. is engaged in the designing, marketing and distributing of athletic footwear, apparel, equipment and accessories and services for sports and fitness activities. The Company's operating segments include North America; Europe, Middle East &amp; Africa (EMEA); Greater China; and Asia Pacific &amp; Latin America (APLA). It sells a line of equipment and accessories under the NIKE Brand name, including bags, socks, sport balls, eyewear, timepieces, digital devices, bats, gloves, protective equipment and other equipment designed for sports activities. It also designs products specifically for the Jordan Brand and Converse. The Jordan Brand designs, distributes and licenses athletic and casual footwear, apparel and accessories predominantly focused on basketball performance and culture using the Jumpman trademark. The Company also designs, distributes and licenses casual sneakers, apparel and accessories under the Chuck Taylor, All Star, One Star, Star Chevron and Jack Purcell trademarks.</v>
     <v>79400</v>
@@ -3232,24 +3232,24 @@
     <v>XFRA</v>
     <v>XFRA</v>
     <v>One Bowerman Dr, BEAVERTON, OR, 97005-6453 US</v>
-    <v>70.3</v>
+    <v>74.5</v>
     <v>Textiles &amp; Apparel</v>
     <v>Stock</v>
-    <v>45665.878472222219</v>
+    <v>45691.878472222219</v>
     <v>71</v>
-    <v>69</v>
-    <v>109121600000</v>
+    <v>71.48</v>
+    <v>113744900000</v>
     <v>NIKE, INC.</v>
     <v>NIKE, INC.</v>
-    <v>69.64</v>
-    <v>22.68</v>
-    <v>69.790000000000006</v>
-    <v>69.14</v>
-    <v>1488496000</v>
+    <v>73</v>
+    <v>24.53</v>
+    <v>74.89</v>
+    <v>74.31</v>
+    <v>1479127000</v>
     <v>NKE</v>
     <v>NIKE, INC. (XFRA:NKE)</v>
-    <v>1697</v>
-    <v>14821070</v>
+    <v>2255</v>
+    <v>11185720</v>
     <v>1969</v>
   </rv>
   <rv s="3">
@@ -3272,12 +3272,12 @@
     <v>Finance</v>
     <v>4</v>
     <v>85.16</v>
-    <v>57.96</v>
-    <v>1.6337999999999999</v>
-    <v>-4.42</v>
-    <v>-2.7439999999999999E-3</v>
-    <v>-7.0460999999999996E-2</v>
-    <v>-0.16</v>
+    <v>49.8</v>
+    <v>1.6129</v>
+    <v>-2.08</v>
+    <v>8.7840000000000001E-3</v>
+    <v>-3.9740000000000004E-2</v>
+    <v>0.4415</v>
     <v>USD</v>
     <v>ON Semiconductor Corporation, together with its wholly owned subsidiaries, operates under the onsemi brand. The Company provides intelligent power and intelligent sensing solutions. Its segments include the Power Solutions Group (PSG), the Analog &amp; Mixed-Signal Group (AMG), and the Intelligent Sensing Group (ISG). PSG offers a range of analog, discrete, module and integrated semiconductor products that perform multiple application functions, including power switching, power conversion, and signal conditioning. AMG designs and develops analog, mixed-signal, power management integrated circuits (ICs) and sensor interface devices for a range of end-users in the automotive, industrial, compute and mobile end-markets. ISG designs and develops complementary metal oxide semiconductor (CMOS) image sensors, image signal processors, and single photon detectors. Its SWIR Vision Systems is a provider of colloidal quantum-dot-based (CQD) short wavelength infrared (SWIR) technology.</v>
     <v>30000</v>
@@ -3285,25 +3285,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>5701 NORTH PIMA ROAD, SCOTTSDALE, AZ, 85250 US</v>
-    <v>62.59</v>
+    <v>51.46</v>
     <v>Semiconductors &amp; Semiconductor Equipment</v>
     <v>Stock</v>
-    <v>45666.041636678128</v>
+    <v>45691.911956018521</v>
     <v>74</v>
-    <v>57.96</v>
-    <v>24828252225</v>
+    <v>49.8</v>
+    <v>21400582350</v>
     <v>ON SEMICONDUCTOR CORPORATION</v>
     <v>ON SEMICONDUCTOR CORPORATION</v>
-    <v>62.41</v>
-    <v>14.596399999999999</v>
-    <v>62.73</v>
-    <v>58.31</v>
-    <v>58.15</v>
+    <v>50.65</v>
+    <v>12.4712</v>
+    <v>52.34</v>
+    <v>50.26</v>
+    <v>50.701500000000003</v>
     <v>425797500</v>
     <v>ON</v>
     <v>ON SEMICONDUCTOR CORPORATION (XNAS:ON)</v>
-    <v>14868262</v>
-    <v>6897303</v>
+    <v>8060450</v>
+    <v>8206634</v>
     <v>2000</v>
   </rv>
   <rv s="3">
@@ -3327,11 +3327,11 @@
     <v>4</v>
     <v>237.72</v>
     <v>107.13</v>
-    <v>1.0516000000000001</v>
-    <v>2.19</v>
-    <v>-2.2980000000000001E-3</v>
-    <v>1.3787000000000001E-2</v>
-    <v>-0.37</v>
+    <v>1.0732999999999999</v>
+    <v>1.1000000000000001</v>
+    <v>1.8790000000000001E-2</v>
+    <v>6.0599999999999994E-3</v>
+    <v>3.43</v>
     <v>USD</v>
     <v>Snowflake Inc. is a data cloud and artificial intelligence company. Its platform is the technology that powers the AI Data Cloud, enabling customers to consolidate data into a single source of truth to drive meaningful insights, apply artificial intelligence (AI) to solve business problems, build data applications, and share data and data products. It provides its platform through a customer-centric, and consumption-based business model. Its cloud-native architecture consists of three independently scalable but logically integrated layers across compute, storage, and cloud services. The compute layer provides dedicated resources to enable users to simultaneously access common data sets for many use cases with minimal latency. The storage layer ingests massive amounts and varieties of structured, semi-structured, and unstructured data to create a unified data record. Its ClearQuery platform allows users to rapidly search, explore, and analyze their data using natural language queries.</v>
     <v>7004</v>
@@ -3339,24 +3339,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>106 East Babcock Street, Suite 3A, BOZEMAN, MT, 59715 US</v>
-    <v>162.58000000000001</v>
+    <v>184.5</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45666.040629120311</v>
+    <v>45691.912040832809</v>
     <v>77</v>
-    <v>156.69999999999999</v>
-    <v>53548820000</v>
+    <v>175.25</v>
+    <v>60279561000</v>
     <v>SNOWFLAKE INC.</v>
     <v>SNOWFLAKE INC.</v>
-    <v>158.30000000000001</v>
-    <v>158.84</v>
-    <v>161.03</v>
-    <v>160.66</v>
+    <v>176.17</v>
+    <v>181.51</v>
+    <v>182.61</v>
+    <v>185.97</v>
     <v>330100000</v>
     <v>SNOW</v>
     <v>SNOWFLAKE INC. (XNYS:SNOW)</v>
-    <v>5407756</v>
-    <v>5330345</v>
+    <v>4356569</v>
+    <v>4793035</v>
     <v>2012</v>
   </rv>
   <rv s="3">
@@ -3378,32 +3378,32 @@
     <v>22</v>
     <v>Finance</v>
     <v>23</v>
-    <v>609.07000000000005</v>
-    <v>468.3</v>
-    <v>0.99829999999999997</v>
-    <v>0.86</v>
-    <v>-2.222E-3</v>
-    <v>1.4610000000000001E-3</v>
-    <v>-1.31</v>
+    <v>610.78</v>
+    <v>490.23</v>
+    <v>0.99819999999999998</v>
+    <v>-4.1100000000000003</v>
+    <v>5.3029999999999996E-3</v>
+    <v>-6.8289999999999991E-3</v>
+    <v>3.17</v>
     <v>USD</v>
     <v>NYSE Arca</v>
     <v>ARCX</v>
-    <v>8.9999999999999998E-4</v>
-    <v>590.57989999999995</v>
+    <v>9.4499999999999998E-4</v>
+    <v>600.29</v>
     <v>ETF</v>
-    <v>45666.041666700781</v>
+    <v>45691.912180428124</v>
     <v>80</v>
-    <v>585.19500000000005</v>
-    <v>623795251613.90002</v>
+    <v>590.49</v>
+    <v>627680565767.93005</v>
     <v>SPDR S&amp;P 500</v>
-    <v>588.70000000000005</v>
-    <v>588.63</v>
-    <v>589.49</v>
-    <v>588.17999999999995</v>
+    <v>592.66999999999996</v>
+    <v>601.82000000000005</v>
+    <v>597.71</v>
+    <v>600.94000000000005</v>
     <v>SPY</v>
     <v>SPDR S&amp;P 500 (ARCX:SPY)</v>
-    <v>47304672</v>
-    <v>47885954</v>
+    <v>65066293</v>
+    <v>44369495</v>
   </rv>
   <rv s="3">
     <v>81</v>
@@ -3423,14 +3423,14 @@
     <v>2</v>
     <v>24</v>
     <v>Finance</v>
-    <v>10</v>
+    <v>4</v>
     <v>29.51</v>
     <v>12.12</v>
-    <v>1.5183</v>
-    <v>-0.34499999999999997</v>
-    <v>2.3493E-2</v>
-    <v>-2.6316000000000003E-2</v>
-    <v>0.3</v>
+    <v>1.4999</v>
+    <v>-0.505</v>
+    <v>1.4215999999999999E-2</v>
+    <v>-3.8462000000000003E-2</v>
+    <v>0.1794</v>
     <v>USD</v>
     <v>Stellantis N.V., formerly Fiat Chrysler Automobiles N.V., is a holding Company based in the Netherlands and operates as an automaker and a mobility provider. The Company is engaged in designing, engineering, manufacturing, distributing and selling vehicles, components and production systems. The Company has industrial operations in more than 30 countries and sells its vehicles directly or through distributors and dealers in more than 130 countries. The Company designs, manufactures, distributes and sells vehicles for the mass-market under the Abarth, Alfa Romeo, Chrysler, Dodge, Fiat, Fiat Professional, Jeep, Lancia and Ram brands. In addition, the Company designs, manufactures, distributes and sells luxury vehicles under the Maserati brand. The Company's brand portfolio also includes Peugeot, Citroen, DS Automobiles, Opel and Vauxhall. It offers a wide variety of vehicle choices from luxury and mainstream passenger vehicles to pickup trucks, sport utility vehicle (SUVs).</v>
     <v>258275</v>
@@ -3438,25 +3438,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>Taurusavenue 1, HOOFDDORP, NOORD-HOLLAND, 2132 LS NL</v>
-    <v>12.850099999999999</v>
+    <v>12.865</v>
     <v>Automobiles &amp; Auto Parts</v>
     <v>Stock</v>
-    <v>45666.035465624998</v>
+    <v>45691.91071083281</v>
     <v>83</v>
-    <v>12.715</v>
-    <v>35262590000</v>
+    <v>12.39</v>
+    <v>37538910000</v>
     <v>Stellantis NV</v>
     <v>Stellantis NV</v>
-    <v>12.84</v>
-    <v>2.7031000000000001</v>
-    <v>13.11</v>
-    <v>12.765000000000001</v>
-    <v>13.07</v>
+    <v>12.52</v>
+    <v>2.6734</v>
+    <v>13.13</v>
+    <v>12.625</v>
+    <v>12.7994</v>
     <v>2896073000</v>
     <v>STLA</v>
     <v>Stellantis NV (XNYS:STLA)</v>
-    <v>9259138</v>
-    <v>9411526</v>
+    <v>18092742</v>
+    <v>8350346</v>
     <v>2014</v>
   </rv>
   <rv s="3">
@@ -3478,13 +3478,13 @@
     <v>3</v>
     <v>Finance</v>
     <v>4</v>
-    <v>192.14</v>
+    <v>192.5</v>
     <v>135.24</v>
-    <v>0.88900000000000001</v>
-    <v>1.99</v>
-    <v>-2.1770000000000001E-4</v>
-    <v>1.0949E-2</v>
-    <v>-0.04</v>
+    <v>0.88739999999999997</v>
+    <v>0.56000000000000005</v>
+    <v>3.3860000000000001E-3</v>
+    <v>3.019E-3</v>
+    <v>0.63</v>
     <v>USD</v>
     <v>Take-Two Interactive Software, Inc. is a developer, publisher, and marketer of interactive entertainment for consumers around the globe. The Company develops, operates and publishes products principally through Rockstar Games, 2K, Private Division, and Zynga. Its products are designed for console gaming systems, including Sony's PlayStation 4 and PlayStation 5; Microsoft Corporation Xbox One and Xbox Series XS; and Nintendo's Switch, as well as personal computers (PC), and mobile, including smartphones and tablets. The Company delivers its products through physical retail, digital download, online platforms, and cloud streaming services. The Company is focused on publishing a select number of titles based on internally owned and developed intellectual properties. In addition, the Company selectively develops titles based on licensed properties, including sports leagues, and also publishes externally developed titles.</v>
     <v>12371</v>
@@ -3492,25 +3492,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>110 West 44Th Street, NEW YORK, NY, 10036 US</v>
-    <v>183.91</v>
+    <v>187.59</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45666.039326376565</v>
+    <v>45691.911738842187</v>
     <v>86</v>
-    <v>180.17</v>
-    <v>32269778476</v>
+    <v>182.89</v>
+    <v>32678990318</v>
     <v>TAKE-TWO INTERACTIVE SOFTWARE, INC.</v>
     <v>TAKE-TWO INTERACTIVE SOFTWARE, INC.</v>
-    <v>181.59</v>
+    <v>184.62</v>
     <v>0</v>
-    <v>181.75</v>
-    <v>183.74</v>
-    <v>183.7</v>
+    <v>185.51</v>
+    <v>186.07</v>
+    <v>186.7</v>
     <v>175627400</v>
     <v>TTWO</v>
     <v>TAKE-TWO INTERACTIVE SOFTWARE, INC. (XNAS:TTWO)</v>
-    <v>1976424</v>
-    <v>1435133</v>
+    <v>1739168</v>
+    <v>1417430</v>
     <v>1993</v>
   </rv>
   <rv s="3">
@@ -3527,14 +3527,14 @@
     <v>26</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>10</v>
     <v>115</v>
-    <v>73.910300000000007</v>
-    <v>0.78800000000000003</v>
-    <v>0.35</v>
-    <v>5.3920000000000001E-3</v>
-    <v>3.4429999999999999E-3</v>
-    <v>0.55000000000000004</v>
+    <v>75.05</v>
+    <v>0.77900000000000003</v>
+    <v>-2.2200000000000002</v>
+    <v>-1.6800000000000001E-3</v>
+    <v>-2.1472000000000002E-2</v>
+    <v>-0.17</v>
     <v>USD</v>
     <v>Veralto Corporation provides essential technology solutions that monitor, enhance, and protect key resources around the globe. The Company operates through two segments: Water Quality (WQ) and Product Quality &amp; Innovation (PQI). The WQ segment provides a comprehensive portfolio of water analytics and differentiated water treatment solutions that enable the reliable delivery of safe drinking water by public and private utilities from source water to the consumer and back into the water cycle. It provides proprietary precision instrumentation and advanced water treatment technologies under Hach, Trojan Technologies, ChemTreat, and other global WQ brands. Its PQI segment provides a broad set of solutions for brand owners and consumer packaged goods companies that enable speed to market as well as traceability and quality control of their products. The brands in this segment include Videojet, Linx, Esko, X-Rite, Pantone and others. TraceGains is complementary to its PQI segment.</v>
     <v>16000</v>
@@ -3542,24 +3542,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>225 Wyman Street, Suite 250, WALTHAM, MA, 02451 US</v>
-    <v>102.05</v>
+    <v>102.59</v>
     <v>Professional &amp; Commercial Services</v>
     <v>Stock</v>
-    <v>45666.000000022657</v>
-    <v>100.2</v>
-    <v>24928620000</v>
+    <v>45691.898595346873</v>
+    <v>100.49</v>
+    <v>25020130126</v>
     <v>VERALTO CORPORATION</v>
     <v>VERALTO CORPORATION</v>
-    <v>101.65</v>
-    <v>31.476600000000001</v>
-    <v>101.65</v>
-    <v>102</v>
-    <v>102.55</v>
+    <v>102.02</v>
+    <v>31.220500000000001</v>
+    <v>103.39</v>
+    <v>101.17</v>
+    <v>101</v>
     <v>247307800</v>
     <v>VLTO</v>
     <v>VERALTO CORPORATION (XNYS:VLTO)</v>
-    <v>1034931</v>
-    <v>1234283</v>
+    <v>1484369</v>
+    <v>1146142</v>
     <v>2022</v>
   </rv>
   <rv s="3">
@@ -3580,14 +3580,14 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>10</v>
-    <v>96.18</v>
-    <v>52.224899999999998</v>
-    <v>0.5464</v>
-    <v>0.97</v>
-    <v>7.6139999999999997E-4</v>
-    <v>1.0682000000000001E-2</v>
-    <v>6.9900000000000004E-2</v>
+    <v>4</v>
+    <v>99.79</v>
+    <v>55.846600000000002</v>
+    <v>0.55210000000000004</v>
+    <v>1.38</v>
+    <v>1.9089999999999999E-3</v>
+    <v>1.4058999999999999E-2</v>
+    <v>0.19</v>
     <v>USD</v>
     <v>Walmart Inc. is a technology-powered omnichannel retailer. The Company is engaged in the operation of retail and wholesale stores and clubs, as well as e-commerce websites and mobile applications, located throughout the United States, Africa, Canada, Central America, Chile, China, India and Mexico. It operates through three segments: Walmart U.S., Walmart International and Sam's Club. The Walmart U.S. segment includes the Company's mass merchant concept in the United States, as well as e-commerce, which includes omni-channel initiatives and certain other business offerings such as advertising services through Walmart Connect. It operates under the Walmart and Walmart Neighborhood Market brands. The Walmart International segment consists of the Company's operations outside of the United States, as well as e-commerce and omni-channel initiatives. The Sam's Club segment includes the warehouse membership clubs in the United States, as well as e-commerce and omni-channel initiatives.</v>
     <v>2100000</v>
@@ -3595,25 +3595,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>702 SW 8th St, BENTONVILLE, AR, 72716-6209 US</v>
-    <v>91.844999999999999</v>
+    <v>99.79</v>
     <v>Food &amp; Drug Retailing</v>
     <v>Stock</v>
-    <v>45666.041661203126</v>
+    <v>45691.912199617967</v>
     <v>91</v>
-    <v>90.82</v>
-    <v>729270800000</v>
+    <v>96.47</v>
+    <v>799643242440</v>
     <v>WALMART INC.</v>
     <v>WALMART INC.</v>
-    <v>91.11</v>
-    <v>46.339500000000001</v>
-    <v>90.81</v>
-    <v>91.78</v>
-    <v>91.869900000000001</v>
+    <v>96.77</v>
+    <v>50.2575</v>
+    <v>98.16</v>
+    <v>99.54</v>
+    <v>99.73</v>
     <v>8033386000</v>
     <v>WMT</v>
     <v>WALMART INC. (XNYS:WMT)</v>
-    <v>13453627</v>
-    <v>17341792</v>
+    <v>20430636</v>
+    <v>14171463</v>
     <v>1969</v>
   </rv>
   <rv s="3">
@@ -3635,13 +3635,13 @@
     <v>19</v>
     <v>Finance</v>
     <v>4</v>
-    <v>16.559999999999999</v>
+    <v>16.86</v>
     <v>8.1</v>
-    <v>1.6990000000000001</v>
-    <v>-0.12</v>
-    <v>4.5570000000000006E-2</v>
-    <v>-7.5380000000000004E-3</v>
-    <v>0.72</v>
+    <v>1.631</v>
+    <v>4.4999999999999998E-2</v>
+    <v>2.4405E-2</v>
+    <v>2.7569999999999999E-3</v>
+    <v>0.4</v>
     <v>USD</v>
     <v>Weave Communications, Inc. offers customer communications and engagement software platform for small and medium-sized businesses. The Company's products feature Customized Phone System, Text Messaging, Missed Call Text, Team Chat, Weave Reviews, Weave Email Marketing and Email Assistant, Text Connect and Digital Forms. Its cloud-based software platform streamlines the day-to-day operations of running a small business. It offers an all-in-one platform spanning all forms of communications and customer engagement ranging from answering phones, to scheduling appointments, to sending text reminders, to requesting client reviews, to collecting payments, to sending email marketing campaigns, and to verify insurance. Its customer base consists of dental and optometry service providers as well as various client service small businesses in other industries such as veterinary, optometry, veterinary, physical therapy, home services, audiology, medical specialty services and podiatry.</v>
     <v>844</v>
@@ -3649,24 +3649,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>1331 W Powell Way, LEHI, UT, 84043 US</v>
-    <v>16.03</v>
+    <v>16.399999999999999</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45666.000000010936</v>
+    <v>45691.90439241875</v>
     <v>94</v>
-    <v>15.71</v>
-    <v>1160699000</v>
+    <v>15.721</v>
+    <v>1187624000</v>
     <v>Weave Communications, Inc.</v>
     <v>Weave Communications, Inc.</v>
-    <v>15.8</v>
-    <v>15.92</v>
-    <v>15.8</v>
-    <v>16.52</v>
+    <v>15.86</v>
+    <v>16.32</v>
+    <v>16.364999999999998</v>
+    <v>16.79</v>
     <v>72771110</v>
     <v>WEAV</v>
     <v>Weave Communications, Inc. (XNYS:WEAV)</v>
-    <v>405802</v>
-    <v>1009993</v>
+    <v>686271</v>
+    <v>713123</v>
     <v>2015</v>
   </rv>
   <rv s="3">
@@ -3792,6 +3792,328 @@
   <rv s="14">
     <fb>11.54</fb>
     <v>27</v>
+  </rv>
+  <rv s="15">
+    <v>29</v>
+    <v>DHR</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638397504000000000,638742164187774965,0</v>
+    <v>0</v>
+    <v>a1r1r7</v>
+    <v>XNYS:DHR</v>
+    <v>1</v>
+  </rv>
+  <rv s="15">
+    <v>29</v>
+    <v>WMT</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638397504000000000,638742162253788087,0</v>
+    <v>0</v>
+    <v>a25ya2</v>
+    <v>XNYS:WMT</v>
+    <v>2</v>
+  </rv>
+  <rv s="15">
+    <v>29</v>
+    <v>NKE</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638397504000000000,638742160509456283,0</v>
+    <v>0</v>
+    <v>a1yjxm</v>
+    <v>XNYS:NKE</v>
+    <v>3</v>
+  </rv>
+  <rv s="15">
+    <v>29</v>
+    <v>SPY</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638397504000000000,638742162343168567,0</v>
+    <v>0</v>
+    <v>a23hqh</v>
+    <v>ARCX:SPY</v>
+    <v>4</v>
+  </rv>
+  <rv s="15">
+    <v>30</v>
+    <v>BRKB</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638397504000000000,638742162253956941,0</v>
+    <v>0</v>
+    <v>b11ibh</v>
+    <v>XWBO:BRKB</v>
+    <v>5</v>
+  </rv>
+  <rv s="15">
+    <v>29</v>
+    <v>AAPL</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638397504000000000,638742160509515399,0</v>
+    <v>0</v>
+    <v>a1mou2</v>
+    <v>XNAS:AAPL</v>
+    <v>6</v>
+  </rv>
+  <rv s="15">
+    <v>29</v>
+    <v>HD</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638397504000000000,638742162518091414,0</v>
+    <v>0</v>
+    <v>a1uj52</v>
+    <v>XNYS:HD</v>
+    <v>7</v>
+  </rv>
+  <rv s="15">
+    <v>29</v>
+    <v>GOOG</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638397504000000000,638742162264893216,0</v>
+    <v>0</v>
+    <v>a1u3p2</v>
+    <v>XNAS:GOOG</v>
+    <v>8</v>
+  </rv>
+  <rv s="15">
+    <v>29</v>
+    <v>COST</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638397504000000000,638742162254123292,0</v>
+    <v>0</v>
+    <v>a1q6k2</v>
+    <v>XNAS:COST</v>
+    <v>9</v>
+  </rv>
+  <rv s="15">
+    <v>29</v>
+    <v>AMZN</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638397504000000000,638742164188439979,0</v>
+    <v>0</v>
+    <v>a1nhlh</v>
+    <v>XNAS:AMZN</v>
+    <v>10</v>
+  </rv>
+  <rv s="15">
+    <v>29</v>
+    <v>MSFT</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638397504000000000,638742162262303506,0</v>
+    <v>0</v>
+    <v>a1xzim</v>
+    <v>XNAS:MSFT</v>
+    <v>11</v>
+  </rv>
+  <rv s="15">
+    <v>29</v>
+    <v>LMT</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638397504000000000,638742162343073522,0</v>
+    <v>0</v>
+    <v>a1wzw7</v>
+    <v>XNYS:LMT</v>
+    <v>12</v>
+  </rv>
+  <rv s="15">
+    <v>29</v>
+    <v>ALL</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638397504000000000,638742162263289808,0</v>
+    <v>0</v>
+    <v>a1nanm</v>
+    <v>XNYS:ALL</v>
+    <v>13</v>
+  </rv>
+  <rv s="15">
+    <v>29</v>
+    <v>HON</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638397504000000000,638742162263923007,0</v>
+    <v>0</v>
+    <v>a1ut3m</v>
+    <v>XNAS:HON</v>
+    <v>14</v>
+  </rv>
+  <rv s="15">
+    <v>29</v>
+    <v>NEE</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638397504000000000,638742162264572528,0</v>
+    <v>0</v>
+    <v>a1ye2w</v>
+    <v>XNYS:NEE</v>
+    <v>15</v>
+  </rv>
+  <rv s="15">
+    <v>29</v>
+    <v>WEAV</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638397504000000000,638742162343013180,0</v>
+    <v>0</v>
+    <v>c3u6sm</v>
+    <v>XNYS:WEAV</v>
+    <v>16</v>
+  </rv>
+  <rv s="15">
+    <v>29</v>
+    <v>CAT</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638397504000000000,638742162343108412,0</v>
+    <v>0</v>
+    <v>a1p7zr</v>
+    <v>XNYS:CAT</v>
+    <v>17</v>
+  </rv>
+  <rv s="15">
+    <v>29</v>
+    <v>ON</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638397504000000000,638742162343138697,0</v>
+    <v>0</v>
+    <v>a1z8jc</v>
+    <v>XNAS:ON</v>
+    <v>18</v>
+  </rv>
+  <rv s="15">
+    <v>29</v>
+    <v>STLA</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638397504000000000,638742162518057746,0</v>
+    <v>0</v>
+    <v>a1snf2</v>
+    <v>XNYS:STLA</v>
+    <v>19</v>
+  </rv>
+  <rv s="15">
+    <v>29</v>
+    <v>ADP</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638397504000000000,638742162517438263,0</v>
+    <v>0</v>
+    <v>a1mw4c</v>
+    <v>XNAS:ADP</v>
+    <v>20</v>
+  </rv>
+  <rv s="15">
+    <v>29</v>
+    <v>SNOW</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638397504000000000,638742164185777123,0</v>
+    <v>0</v>
+    <v>bvlqa2</v>
+    <v>XNYS:SNOW</v>
+    <v>21</v>
+  </rv>
+  <rv s="15">
+    <v>29</v>
+    <v>DG</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638397504000000000,638742164186114779,0</v>
+    <v>0</v>
+    <v>a1qyvh</v>
+    <v>XNYS:DG</v>
+    <v>22</v>
+  </rv>
+  <rv s="15">
+    <v>29</v>
+    <v>VLTO</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638397504000000000,638742164186452939,0</v>
+    <v>0</v>
+    <v>caydcw</v>
+    <v>XNYS:VLTO</v>
+    <v>23</v>
   </rv>
   <rv s="15">
     <v>29</v>
@@ -3801,11 +4123,25 @@
     <v>45293</v>
     <v>0</v>
     <v>1</v>
-    <v>638397504000000000,638682484997389055,0</v>
+    <v>638397504000000000,638742164186780679,0</v>
     <v>0</v>
     <v>a24mnm</v>
     <v>XNAS:TTWO</v>
+    <v>24</v>
+  </rv>
+  <rv s="15">
+    <v>29</v>
+    <v>ADBE</v>
+    <v>Daily</v>
+    <v>45293</v>
+    <v>45293</v>
+    <v>0</v>
     <v>1</v>
+    <v>638397504000000000,638742164187111274,0</v>
+    <v>0</v>
+    <v>a1mv7w</v>
+    <v>XNAS:ADBE</v>
+    <v>25</v>
   </rv>
   <rv s="15">
     <v>29</v>
@@ -3815,95 +4151,25 @@
     <v>45293</v>
     <v>0</v>
     <v>1</v>
-    <v>638397504000000000,638682484997401215,0</v>
+    <v>638397504000000000,638742164187442982,0</v>
     <v>0</v>
     <v>a1w8ec</v>
     <v>XNYS:JNJ</v>
-    <v>2</v>
+    <v>26</v>
   </rv>
   <rv s="15">
     <v>29</v>
-    <v>SNOW</v>
+    <v>MA</v>
     <v>Daily</v>
     <v>45293</v>
     <v>45293</v>
     <v>0</v>
     <v>1</v>
-    <v>638397504000000000,638682484997453923,0</v>
+    <v>638397504000000000,638742164188773992,0</v>
     <v>0</v>
-    <v>bvlqa2</v>
-    <v>XNYS:SNOW</v>
-    <v>3</v>
-  </rv>
-  <rv s="15">
-    <v>29</v>
-    <v>DG</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638682484997441939,0</v>
-    <v>0</v>
-    <v>a1qyvh</v>
-    <v>XNYS:DG</v>
-    <v>4</v>
-  </rv>
-  <rv s="15">
-    <v>29</v>
-    <v>VLTO</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638717178408054771,0</v>
-    <v>0</v>
-    <v>caydcw</v>
-    <v>XNYS:VLTO</v>
-    <v>5</v>
-  </rv>
-  <rv s="15">
-    <v>29</v>
-    <v>ADBE</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638682484997511661,0</v>
-    <v>0</v>
-    <v>a1mv7w</v>
-    <v>XNAS:ADBE</v>
-    <v>6</v>
-  </rv>
-  <rv s="15">
-    <v>29</v>
-    <v>SPY</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638693606240233000,0</v>
-    <v>0</v>
-    <v>a23hqh</v>
-    <v>ARCX:SPY</v>
-    <v>7</v>
-  </rv>
-  <rv s="15">
-    <v>30</v>
-    <v>BRKB</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638689196879322825,0</v>
-    <v>0</v>
-    <v>b11ibh</v>
-    <v>XWBO:BRKB</v>
-    <v>8</v>
+    <v>a1x8w7</v>
+    <v>XNYS:MA</v>
+    <v>27</v>
   </rv>
   <rv s="15">
     <v>29</v>
@@ -3913,276 +4179,10 @@
     <v>45293</v>
     <v>0</v>
     <v>1</v>
-    <v>638397504000000000,638682484997622113,0</v>
+    <v>638397504000000000,638742164185189598,0</v>
     <v>0</v>
     <v>a1r2z2</v>
     <v>XNYS:DIS</v>
-    <v>9</v>
-  </rv>
-  <rv s="15">
-    <v>29</v>
-    <v>LMT</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638693606240298858,0</v>
-    <v>0</v>
-    <v>a1wzw7</v>
-    <v>XNYS:LMT</v>
-    <v>10</v>
-  </rv>
-  <rv s="15">
-    <v>29</v>
-    <v>AMZN</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638682484998239239,0</v>
-    <v>0</v>
-    <v>a1nhlh</v>
-    <v>XNAS:AMZN</v>
-    <v>11</v>
-  </rv>
-  <rv s="15">
-    <v>29</v>
-    <v>MSFT</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638689196879269862,0</v>
-    <v>0</v>
-    <v>a1xzim</v>
-    <v>XNAS:MSFT</v>
-    <v>12</v>
-  </rv>
-  <rv s="15">
-    <v>29</v>
-    <v>DHR</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638682485001056102,0</v>
-    <v>0</v>
-    <v>a1r1r7</v>
-    <v>XNYS:DHR</v>
-    <v>13</v>
-  </rv>
-  <rv s="15">
-    <v>29</v>
-    <v>WMT</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638689196880816118,0</v>
-    <v>0</v>
-    <v>a25ya2</v>
-    <v>XNYS:WMT</v>
-    <v>14</v>
-  </rv>
-  <rv s="15">
-    <v>29</v>
-    <v>ON</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638682485000974287,0</v>
-    <v>0</v>
-    <v>a1z8jc</v>
-    <v>XNAS:ON</v>
-    <v>15</v>
-  </rv>
-  <rv s="15">
-    <v>29</v>
-    <v>ADP</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638682485001026209,0</v>
-    <v>0</v>
-    <v>a1mw4c</v>
-    <v>XNAS:ADP</v>
-    <v>16</v>
-  </rv>
-  <rv s="15">
-    <v>29</v>
-    <v>AAPL</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638682484996833420,0</v>
-    <v>0</v>
-    <v>a1mou2</v>
-    <v>XNAS:AAPL</v>
-    <v>17</v>
-  </rv>
-  <rv s="15">
-    <v>29</v>
-    <v>ALL</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638682484996980917,0</v>
-    <v>0</v>
-    <v>a1nanm</v>
-    <v>XNYS:ALL</v>
-    <v>18</v>
-  </rv>
-  <rv s="15">
-    <v>29</v>
-    <v>COST</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638682484997004104,0</v>
-    <v>0</v>
-    <v>a1q6k2</v>
-    <v>XNAS:COST</v>
-    <v>19</v>
-  </rv>
-  <rv s="15">
-    <v>29</v>
-    <v>MA</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638689196880846132,0</v>
-    <v>0</v>
-    <v>a1x8w7</v>
-    <v>XNYS:MA</v>
-    <v>20</v>
-  </rv>
-  <rv s="15">
-    <v>29</v>
-    <v>NEE</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638689196880976898,0</v>
-    <v>0</v>
-    <v>a1ye2w</v>
-    <v>XNYS:NEE</v>
-    <v>21</v>
-  </rv>
-  <rv s="15">
-    <v>29</v>
-    <v>STLA</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638689196880190375,0</v>
-    <v>0</v>
-    <v>a1snf2</v>
-    <v>XNYS:STLA</v>
-    <v>22</v>
-  </rv>
-  <rv s="15">
-    <v>29</v>
-    <v>HON</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638693606240201827,0</v>
-    <v>0</v>
-    <v>a1ut3m</v>
-    <v>XNAS:HON</v>
-    <v>23</v>
-  </rv>
-  <rv s="15">
-    <v>29</v>
-    <v>GOOG</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638693606240410922,0</v>
-    <v>0</v>
-    <v>a1u3p2</v>
-    <v>XNAS:GOOG</v>
-    <v>24</v>
-  </rv>
-  <rv s="15">
-    <v>29</v>
-    <v>HD</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638693606240272150,0</v>
-    <v>0</v>
-    <v>a1uj52</v>
-    <v>XNYS:HD</v>
-    <v>25</v>
-  </rv>
-  <rv s="15">
-    <v>29</v>
-    <v>NKE</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638693606240321300,0</v>
-    <v>0</v>
-    <v>a1yjxm</v>
-    <v>XNYS:NKE</v>
-    <v>26</v>
-  </rv>
-  <rv s="15">
-    <v>29</v>
-    <v>CAT</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638693606240351165,0</v>
-    <v>0</v>
-    <v>a1p7zr</v>
-    <v>XNYS:CAT</v>
-    <v>27</v>
-  </rv>
-  <rv s="15">
-    <v>29</v>
-    <v>WEAV</v>
-    <v>Daily</v>
-    <v>45293</v>
-    <v>45293</v>
-    <v>0</v>
-    <v>1</v>
-    <v>638397504000000000,638693606240392901,0</v>
-    <v>0</v>
-    <v>c3u6sm</v>
-    <v>XNYS:WEAV</v>
     <v>28</v>
   </rv>
 </rvData>
@@ -4914,9 +4914,9 @@
       <v>at close</v>
       <v>from previous close</v>
       <v>from previous close</v>
-      <v>Source: Nasdaq</v>
+      <v>Source: Nasdaq Last Sale</v>
       <v>GMT</v>
-      <v>Delayed 15 minutes</v>
+      <v>Real-Time Nasdaq Last Sale</v>
       <v>from close</v>
       <v>from close</v>
     </spb>
@@ -4969,9 +4969,9 @@
       <v>at close</v>
       <v>from previous close</v>
       <v>from previous close</v>
-      <v>Source: Nasdaq Last Sale</v>
+      <v>Source: Nasdaq</v>
       <v>GMT</v>
-      <v>Real-Time Nasdaq Last Sale</v>
+      <v>Delayed 15 minutes</v>
       <v>from close</v>
       <v>from close</v>
     </spb>
@@ -5122,10 +5122,10 @@
     <spb s="16">
       <v>at close</v>
       <v>from previous close</v>
-      <v>Source: Nasdaq</v>
+      <v>Source: Nasdaq Last Sale</v>
       <v>from previous close</v>
       <v>GMT</v>
-      <v>Delayed 15 minutes</v>
+      <v>Real-Time Nasdaq Last Sale</v>
       <v>from close</v>
       <v>from close</v>
     </spb>
@@ -5898,19 +5898,19 @@
     <row r="7" spans="2:16">
       <c r="B7" s="65">
         <f ca="1">SUM(Transaction!G6:G34)</f>
-        <v>1078836.7822251385</v>
+        <v>1105661.0689377724</v>
       </c>
       <c r="C7" s="65"/>
       <c r="D7" s="65"/>
       <c r="F7" s="66">
         <f ca="1">SUMPRODUCT(Transaction!I6:I34,Transaction!H6:H34)</f>
-        <v>6.5260366508605391E-4</v>
+        <v>-3.8124458278748856E-3</v>
       </c>
       <c r="G7" s="66"/>
       <c r="H7" s="66"/>
       <c r="J7" s="66">
         <f ca="1">Transaction!G3</f>
-        <v>0.22752716852603441</v>
+        <v>0.2683590553868721</v>
       </c>
       <c r="K7" s="67"/>
       <c r="L7" s="67"/>
@@ -5957,19 +5957,19 @@
     <row r="12" spans="2:16">
       <c r="B12" s="64" cm="1">
         <f t="array" aca="1" ref="B12" ca="1">SUMPRODUCT(Transaction!H6:H34*Portfolio!F6:F34)</f>
-        <v>1.1911209661589718E-2</v>
+        <v>1.1866760924519295E-2</v>
       </c>
       <c r="C12" s="64"/>
       <c r="D12" s="64"/>
       <c r="F12" s="66">
         <f ca="1">Transaction!I29</f>
-        <v>1.4610000000000001E-3</v>
+        <v>-6.8289999999999991E-3</v>
       </c>
       <c r="G12" s="67"/>
       <c r="H12" s="67"/>
       <c r="J12" s="66">
         <f ca="1">Transaction!H3</f>
-        <v>0.24720194647201954</v>
+        <v>0.26459325081984569</v>
       </c>
       <c r="K12" s="67"/>
       <c r="L12" s="67"/>
@@ -6080,23 +6080,23 @@
       <c r="C3" s="71"/>
       <c r="D3" s="19">
         <f ca="1">SUM(Table1[Total Value])</f>
-        <v>1078836.7822251385</v>
+        <v>1105661.0689377724</v>
       </c>
       <c r="E3" s="20">
         <f ca="1">SUMPRODUCT(Table1[Weight],Table1[Day Change])</f>
-        <v>6.5260366508605391E-4</v>
+        <v>-3.8124458278748856E-3</v>
       </c>
       <c r="F3" s="19">
         <f ca="1">SUMPRODUCT(Table1[Total Value],Table1[Day Change])</f>
-        <v>704.05283810977039</v>
+        <v>-4215.2729293154989</v>
       </c>
       <c r="G3" s="27">
         <f ca="1">(J6*H6)+SUMPRODUCT(J7:J13,H7:H13)+(K14*H14)+SUMPRODUCT(J15:J20,H15:H20)+(K21*H21)+SUMPRODUCT(J22:J24,H22:H24)+(K25*H25)+(J26*H26)+(K27*H27)+(K28*H28)+(J29*H29)+(J30*H30)+(K31*H31)+(J32*H32)+(H33*J33)+(K34*H34)</f>
-        <v>0.22752716852603441</v>
+        <v>0.2683590553868721</v>
       </c>
       <c r="H3" s="27">
         <f ca="1">J29</f>
-        <v>0.24720194647201954</v>
+        <v>0.26459325081984569</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -6147,7 +6147,7 @@
       </c>
       <c r="C6" s="6" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">_FV(A6,"Price")</f>
-        <v>242.7</v>
+        <v>228.01</v>
       </c>
       <c r="D6" s="7">
         <f>164.75</f>
@@ -6162,23 +6162,23 @@
       </c>
       <c r="G6" s="10">
         <f ca="1">C6*F6</f>
-        <v>19901.399999999998</v>
+        <v>18696.82</v>
       </c>
       <c r="H6" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>1.8447090725765454E-2</v>
+        <v>1.6910082596977349E-2</v>
       </c>
       <c r="I6" s="11" cm="1">
         <f t="array" aca="1" ref="I6" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>2.0230000000000001E-3</v>
+        <v>-3.3856000000000004E-2</v>
       </c>
       <c r="J6" s="11">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B2)/'YTD Calculation'!B2</f>
-        <v>0.30736910148674856</v>
+        <v>0.22823744882568417</v>
       </c>
       <c r="K6" s="25">
         <f ca="1">(G6-E6)/E6</f>
-        <v>0.47314112291350513</v>
+        <v>0.38397572078907433</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -6191,7 +6191,7 @@
       </c>
       <c r="C7" s="6" cm="1">
         <f t="array" aca="1" ref="C7" ca="1">_FV(A7,"Price")</f>
-        <v>419.58</v>
+        <v>438.6</v>
       </c>
       <c r="D7" s="12">
         <v>195.01</v>
@@ -6205,23 +6205,23 @@
       </c>
       <c r="G7" s="10">
         <f t="shared" ref="G7:G34" ca="1" si="0">C7*F7</f>
-        <v>20139.603325983284</v>
+        <v>21052.552597302707</v>
       </c>
       <c r="H7" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>1.8667887170517723E-2</v>
+        <v>1.9040692657767408E-2</v>
       </c>
       <c r="I7" s="15" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>-7.2170000000000003E-3</v>
+        <v>2.6290000000000003E-3</v>
       </c>
       <c r="J7" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B3)/'YTD Calculation'!B3</f>
-        <v>-0.27667350492181986</v>
+        <v>-0.24388435878428469</v>
       </c>
       <c r="K7" s="25">
         <f t="shared" ref="K7:K34" ca="1" si="1">(G7-E7)/E7</f>
-        <v>1.1515819701553767</v>
+        <v>1.2491154299779501</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -6234,7 +6234,7 @@
       </c>
       <c r="C8" s="6" cm="1">
         <f t="array" aca="1" ref="C8" ca="1">_FV(A8,"Price")</f>
-        <v>291.89</v>
+        <v>307.32</v>
       </c>
       <c r="D8" s="12">
         <v>118</v>
@@ -6248,23 +6248,23 @@
       </c>
       <c r="G8" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43199.274744067792</v>
+        <v>45482.891206779655</v>
       </c>
       <c r="H8" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>4.0042456334282356E-2</v>
+        <v>4.1136377579501691E-2</v>
       </c>
       <c r="I8" s="15" cm="1">
         <f t="array" aca="1" ref="I8" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>1.2100999999999999E-2</v>
+        <v>1.4224000000000001E-2</v>
       </c>
       <c r="J8" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B4)/'YTD Calculation'!B4</f>
-        <v>0.25049267414960158</v>
+        <v>0.31659669265701312</v>
       </c>
       <c r="K8" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>1.4736440677966101</v>
+        <v>1.6044067796610166</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -6277,7 +6277,7 @@
       </c>
       <c r="C9" s="6" cm="1">
         <f t="array" aca="1" ref="C9" ca="1">_FV(A9,"Price")</f>
-        <v>191.8</v>
+        <v>191.98</v>
       </c>
       <c r="D9" s="12">
         <v>116.85</v>
@@ -6291,23 +6291,23 @@
       </c>
       <c r="G9" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>5754</v>
+        <v>5759.4</v>
       </c>
       <c r="H9" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>5.3335222665769465E-3</v>
+        <v>5.2090103936942942E-3</v>
       </c>
       <c r="I9" s="15" cm="1">
         <f t="array" aca="1" ref="I9" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>3.0960999999999999E-2</v>
+        <v>-1.82E-3</v>
       </c>
       <c r="J9" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B5)/'YTD Calculation'!B5</f>
-        <v>0.33370419303247345</v>
+        <v>0.33495584451707106</v>
       </c>
       <c r="K9" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.64142062473256312</v>
+        <v>0.6429610611895592</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -6320,7 +6320,7 @@
       </c>
       <c r="C10" s="6" cm="1">
         <f t="array" aca="1" ref="C10" ca="1">_FV(A10,"Price")</f>
-        <v>222.13</v>
+        <v>237.42</v>
       </c>
       <c r="D10" s="12">
         <v>68.48</v>
@@ -6334,23 +6334,23 @@
       </c>
       <c r="G10" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44427.784046436907</v>
+        <v>47485.906848714942</v>
       </c>
       <c r="H10" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>4.1181191426197993E-2</v>
+        <v>4.2947977624223914E-2</v>
       </c>
       <c r="I10" s="15" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>9.0050000000000007E-5</v>
+        <v>-1.0939999999999999E-3</v>
       </c>
       <c r="J10" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B6)/'YTD Calculation'!B6</f>
-        <v>0.48155806042819971</v>
+        <v>0.58353898485960098</v>
       </c>
       <c r="K10" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>2.243720794392523</v>
+        <v>2.4669976635514015</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -6363,7 +6363,7 @@
       </c>
       <c r="C11" s="16" cm="1">
         <f t="array" aca="1" ref="C11" ca="1">_FV(A11,"Price")</f>
-        <v>440.15</v>
+        <v>450.15</v>
       </c>
       <c r="D11" s="12">
         <v>103.38</v>
@@ -6377,20 +6377,20 @@
       </c>
       <c r="G11" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>47534.198931127881</v>
+        <v>48614.153467788739</v>
       </c>
       <c r="H11" s="47">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>4.4060602784683461E-2</v>
+        <v>4.3968404815494855E-2</v>
       </c>
       <c r="I11" s="15" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>2.163E-3</v>
+        <v>-6.2909999999999997E-3</v>
       </c>
       <c r="J11" s="62"/>
       <c r="K11" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>3.2575933449409948</v>
+        <v>3.3543238537434705</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -6403,7 +6403,7 @@
       </c>
       <c r="C12" s="6" cm="1">
         <f t="array" aca="1" ref="C12" ca="1">_FV(A12,"Price")</f>
-        <v>361.07</v>
+        <v>361.51</v>
       </c>
       <c r="D12" s="12">
         <v>275.18</v>
@@ -6417,23 +6417,23 @@
       </c>
       <c r="G12" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>35745.93</v>
+        <v>35789.49</v>
       </c>
       <c r="H12" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>3.3133770176312277E-2</v>
+        <v>3.2369313712368994E-2</v>
       </c>
       <c r="I12" s="15" cm="1">
         <f t="array" aca="1" ref="I12" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>-5.3169999999999997E-3</v>
+        <v>-2.6734000000000001E-2</v>
       </c>
       <c r="J12" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B8)/'YTD Calculation'!B8</f>
-        <v>0.2335417307232415</v>
+        <v>0.23504492501110319</v>
       </c>
       <c r="K12" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.31212297405334694</v>
+        <v>0.3137219274656588</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -6446,7 +6446,7 @@
       </c>
       <c r="C13" s="6" cm="1">
         <f t="array" aca="1" ref="C13" ca="1">_FV(A13,"Price")</f>
-        <v>927.37</v>
+        <v>1005.83</v>
       </c>
       <c r="D13" s="12">
         <v>165.95</v>
@@ -6460,23 +6460,23 @@
       </c>
       <c r="G13" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>61732.833100331431</v>
+        <v>66955.730201868049</v>
       </c>
       <c r="H13" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>5.7221661438911373E-2</v>
+        <v>6.0557192509449187E-2</v>
       </c>
       <c r="I13" s="15" cm="1">
         <f t="array" aca="1" ref="I13" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>6.5120000000000004E-3</v>
+        <v>2.6483E-2</v>
       </c>
       <c r="J13" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B9)/'YTD Calculation'!B9</f>
-        <v>0.42529777914393307</v>
+        <v>0.54588488434642291</v>
       </c>
       <c r="K13" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>4.588249472732751</v>
+        <v>5.0610424826755063</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -6506,7 +6506,7 @@
       </c>
       <c r="H14" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>2.3780218331896343E-2</v>
+        <v>2.3203289820488547E-2</v>
       </c>
       <c r="I14" s="15" cm="1">
         <f t="array" aca="1" ref="I14" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
@@ -6531,7 +6531,7 @@
       </c>
       <c r="C15" s="6" cm="1">
         <f t="array" aca="1" ref="C15" ca="1">_FV(A15,"Price")</f>
-        <v>71.62</v>
+        <v>71.47</v>
       </c>
       <c r="D15" s="12">
         <v>62</v>
@@ -6545,23 +6545,23 @@
       </c>
       <c r="G15" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>11551.612903225807</v>
+        <v>11527.419354838708</v>
       </c>
       <c r="H15" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>1.0707470391767884E-2</v>
+        <v>1.042581644473862E-2</v>
       </c>
       <c r="I15" s="15" cm="1">
         <f t="array" aca="1" ref="I15" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>-3.4380000000000001E-2</v>
+        <v>5.77E-3</v>
       </c>
       <c r="J15" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B11)/'YTD Calculation'!B11</f>
-        <v>-0.48999501531011891</v>
+        <v>-0.49106316314177884</v>
       </c>
       <c r="K15" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.15516129032258069</v>
+        <v>0.15274193548387083</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -6574,7 +6574,7 @@
       </c>
       <c r="C16" s="6" cm="1">
         <f t="array" aca="1" ref="C16" ca="1">_FV(A16,"Price")</f>
-        <v>238.09</v>
+        <v>214.2</v>
       </c>
       <c r="D16" s="12">
         <v>74.25</v>
@@ -6588,23 +6588,23 @@
       </c>
       <c r="G16" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>39286.485365656568</v>
+        <v>35344.471272727271</v>
       </c>
       <c r="H16" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>3.6415596884476653E-2</v>
+        <v>3.1966822623756948E-2</v>
       </c>
       <c r="I16" s="15" cm="1">
         <f t="array" aca="1" ref="I16" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>-4.2240000000000003E-3</v>
+        <v>-3.8341E-2</v>
       </c>
       <c r="J16" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B12)/'YTD Calculation'!B12</f>
-        <v>1.4055113079773463E-2</v>
+        <v>-8.7695387367434749E-2</v>
       </c>
       <c r="K16" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2065993265993264</v>
+        <v>1.8848484848484846</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -6617,7 +6617,7 @@
       </c>
       <c r="C17" s="6" cm="1">
         <f t="array" aca="1" ref="C17" ca="1">_FV(A17,"Price")</f>
-        <v>109.76</v>
+        <v>114.06</v>
       </c>
       <c r="D17" s="12">
         <v>101.9</v>
@@ -6631,23 +6631,23 @@
       </c>
       <c r="G17" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>2195.2000000000003</v>
+        <v>2281.1999999999998</v>
       </c>
       <c r="H17" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>2.0347841639884799E-3</v>
+        <v>2.0632000746771233E-3</v>
       </c>
       <c r="I17" s="15" cm="1">
         <f t="array" aca="1" ref="I17" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>-1.4633E-2</v>
+        <v>8.8449999999999987E-3</v>
       </c>
       <c r="J17" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B13)/'YTD Calculation'!B13</f>
-        <v>0.21000992172858574</v>
+        <v>0.25741373608201973</v>
       </c>
       <c r="K17" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>7.7134445534838211E-2</v>
+        <v>0.11933267909715399</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -6660,7 +6660,7 @@
       </c>
       <c r="C18" s="6" cm="1">
         <f t="array" aca="1" ref="C18" ca="1">_FV(A18,"Price")</f>
-        <v>195.39</v>
+        <v>202.64</v>
       </c>
       <c r="D18" s="12">
         <v>25.58</v>
@@ -6674,23 +6674,23 @@
       </c>
       <c r="G18" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>57055.331293979667</v>
+        <v>59172.38514464425</v>
       </c>
       <c r="H18" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>5.2885971477818039E-2</v>
+        <v>5.351765274822616E-2</v>
       </c>
       <c r="I18" s="15" cm="1">
         <f t="array" aca="1" ref="I18" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>-6.7100000000000007E-3</v>
+        <v>-1.4397E-2</v>
       </c>
       <c r="J18" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B14)/'YTD Calculation'!B14</f>
-        <v>0.40004299226139284</v>
+        <v>0.45199197477787317</v>
       </c>
       <c r="K18" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>6.6383893666927278</v>
+        <v>6.9218139171227513</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -6703,7 +6703,7 @@
       </c>
       <c r="C19" s="6" cm="1">
         <f t="array" aca="1" ref="C19" ca="1">_FV(A19,"Price")</f>
-        <v>387.2</v>
+        <v>408.82</v>
       </c>
       <c r="D19" s="12">
         <v>174.29</v>
@@ -6717,23 +6717,23 @@
       </c>
       <c r="G19" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>27104.266590165815</v>
+        <v>28617.681475701414</v>
       </c>
       <c r="H19" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>2.51236026030391E-2</v>
+        <v>2.5882869786846084E-2</v>
       </c>
       <c r="I19" s="15" cm="1">
         <f t="array" aca="1" ref="I19" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>7.7299999999999999E-3</v>
+        <v>-7.6699999999999997E-3</v>
       </c>
       <c r="J19" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B15)/'YTD Calculation'!B15</f>
-        <v>0.12205865306595574</v>
+        <v>0.18471079170047527</v>
       </c>
       <c r="K19" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2215847151299557</v>
+        <v>1.3456308451431522</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -6746,7 +6746,7 @@
       </c>
       <c r="C20" s="6" cm="1">
         <f t="array" aca="1" ref="C20" ca="1">_FV(A20,"Price")</f>
-        <v>220.17</v>
+        <v>222.41</v>
       </c>
       <c r="D20" s="12">
         <v>94.96</v>
@@ -6760,23 +6760,23 @@
       </c>
       <c r="G20" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>25098.869917860149</v>
+        <v>25354.224728306657</v>
       </c>
       <c r="H20" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>2.3264751750577926E-2</v>
+        <v>2.293128105945242E-2</v>
       </c>
       <c r="I20" s="15" cm="1">
         <f t="array" aca="1" ref="I20" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>-2.085E-3</v>
+        <v>-5.8560000000000001E-3</v>
       </c>
       <c r="J20" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B16)/'YTD Calculation'!B16</f>
-        <v>5.3444976076554962E-2</v>
+        <v>6.416267942583731E-2</v>
       </c>
       <c r="K20" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>1.3185551811288962</v>
+        <v>1.3421440606571191</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -6789,7 +6789,7 @@
       </c>
       <c r="C21" s="6" cm="1">
         <f t="array" aca="1" ref="C21" ca="1">_FV(A21,"Price")</f>
-        <v>142.27000000000001</v>
+        <v>151.87</v>
       </c>
       <c r="D21" s="12">
         <v>154.33000000000001</v>
@@ -6803,23 +6803,23 @@
       </c>
       <c r="G21" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>19003.650950560488</v>
+        <v>20285.96661180587</v>
       </c>
       <c r="H21" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>1.7614945340818651E-2</v>
+        <v>1.8347364469742021E-2</v>
       </c>
       <c r="I21" s="15" cm="1">
         <f t="array" aca="1" ref="I21" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>-2.7081000000000001E-2</v>
+        <v>-1.8400000000000001E-3</v>
       </c>
       <c r="J21" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B17)/'YTD Calculation'!B17</f>
-        <v>-0.11064574607738945</v>
+        <v>-5.063449396761889E-2</v>
       </c>
       <c r="K21" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>-7.8144236376595622E-2</v>
+        <v>-1.5939869111643953E-2</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -6832,7 +6832,7 @@
       </c>
       <c r="C22" s="6" cm="1">
         <f t="array" aca="1" ref="C22" ca="1">_FV(A22,"Price")</f>
-        <v>468.85</v>
+        <v>455.4</v>
       </c>
       <c r="D22" s="12">
         <v>312.20999999999998</v>
@@ -6846,23 +6846,23 @@
       </c>
       <c r="G22" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>16256.379991031677</v>
+        <v>15790.029749207262</v>
       </c>
       <c r="H22" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>1.5068433204049946E-2</v>
+        <v>1.4281075994090137E-2</v>
       </c>
       <c r="I22" s="15" cm="1">
         <f t="array" aca="1" ref="I22" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>1.0540000000000001E-2</v>
+        <v>-1.6308E-2</v>
       </c>
       <c r="J22" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B18)/'YTD Calculation'!B18</f>
-        <v>2.7909322108217175E-2</v>
+        <v>-1.5785319652723566E-3</v>
       </c>
       <c r="K22" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.50171359021171658</v>
+        <v>0.45863361199192842</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -6875,7 +6875,7 @@
       </c>
       <c r="C23" s="6" cm="1">
         <f t="array" aca="1" ref="C23" ca="1">_FV(A23,"Price")</f>
-        <v>516.4</v>
+        <v>564.34100000000001</v>
       </c>
       <c r="D23" s="12">
         <v>90.26</v>
@@ -6889,23 +6889,23 @@
       </c>
       <c r="G23" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>50605.99853755816</v>
+        <v>55304.104997451803</v>
       </c>
       <c r="H23" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>4.690792840153403E-2</v>
+        <v>5.0019039786381739E-2</v>
       </c>
       <c r="I23" s="15" cm="1">
         <f t="array" aca="1" ref="I23" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>9.777000000000001E-3</v>
+        <v>1.6043000000000002E-2</v>
       </c>
       <c r="J23" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B19)/'YTD Calculation'!B19</f>
-        <v>0.22401573869966104</v>
+        <v>0.33764962430965423</v>
       </c>
       <c r="K23" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>4.7212497230223782</v>
+        <v>5.2523930866385991</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -6918,7 +6918,7 @@
       </c>
       <c r="C24" s="6" cm="1">
         <f t="array" aca="1" ref="C24" ca="1">_FV(A24,"Price")</f>
-        <v>424.56</v>
+        <v>410.92</v>
       </c>
       <c r="D24" s="12">
         <v>154.66</v>
@@ -6932,23 +6932,23 @@
       </c>
       <c r="G24" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>47549.649403853611</v>
+        <v>46022.003799301696</v>
       </c>
       <c r="H24" s="47">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>4.4074924202881553E-2</v>
+        <v>4.1623970574921142E-2</v>
       </c>
       <c r="I24" s="15" cm="1">
         <f t="array" aca="1" ref="I24" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>5.1849999999999995E-3</v>
+        <v>-9.9740000000000002E-3</v>
       </c>
       <c r="J24" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B20)/'YTD Calculation'!B20</f>
-        <v>0.14476770836142044</v>
+        <v>0.10798932240407692</v>
       </c>
       <c r="K24" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7451183240656925</v>
+        <v>1.6569248674511836</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -6961,7 +6961,7 @@
       </c>
       <c r="C25" s="6" cm="1">
         <f t="array" aca="1" ref="C25" ca="1">_FV(A25,"Price")</f>
-        <v>70.66</v>
+        <v>71.069999999999993</v>
       </c>
       <c r="D25" s="12">
         <v>65.91</v>
@@ -6975,23 +6975,23 @@
       </c>
       <c r="G25" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>22753.581347291758</v>
+        <v>22885.607505689572</v>
       </c>
       <c r="H25" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>2.1090846847436645E-2</v>
+        <v>2.0698574046453647E-2</v>
       </c>
       <c r="I25" s="15" cm="1">
         <f t="array" aca="1" ref="I25" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>3.2659999999999998E-3</v>
+        <v>-6.8469999999999998E-3</v>
       </c>
       <c r="J25" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B21)/'YTD Calculation'!B21</f>
-        <v>0.14763683612148767</v>
+        <v>0.15429592333928849</v>
       </c>
       <c r="K25" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>7.2067971476255419E-2</v>
+        <v>7.8288575329995294E-2</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -7004,7 +7004,7 @@
       </c>
       <c r="C26" s="16" cm="1">
         <f t="array" aca="1" ref="C26" ca="1">_FV(A26,"Price")</f>
-        <v>69.14</v>
+        <v>74.31</v>
       </c>
       <c r="D26" s="12">
         <v>131.91</v>
@@ -7018,23 +7018,23 @@
       </c>
       <c r="G26" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>6151.6883890531426</v>
+        <v>6611.6859153968617</v>
       </c>
       <c r="H26" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>5.702149287462252E-3</v>
+        <v>5.9798487087447351E-3</v>
       </c>
       <c r="I26" s="15" cm="1">
         <f t="array" aca="1" ref="I26" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>-9.3139999999999994E-3</v>
+        <v>-7.7449999999999993E-3</v>
       </c>
       <c r="J26" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B22)/'YTD Calculation'!B22</f>
-        <v>-0.35110276865321444</v>
+        <v>-0.30258094791177848</v>
       </c>
       <c r="K26" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.47585474945038286</v>
+        <v>-0.43666136001819422</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -7047,7 +7047,7 @@
       </c>
       <c r="C27" s="6" cm="1">
         <f t="array" aca="1" ref="C27" ca="1">_FV(A27,"Price")</f>
-        <v>58.31</v>
+        <v>50.26</v>
       </c>
       <c r="D27" s="12">
         <v>71.45</v>
@@ -7061,23 +7061,23 @@
       </c>
       <c r="G27" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>11661.183904828551</v>
+        <v>10051.296571028692</v>
       </c>
       <c r="H27" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>1.0809034412765341E-2</v>
+        <v>9.090757424140063E-3</v>
       </c>
       <c r="I27" s="15" cm="1">
         <f t="array" aca="1" ref="I27" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>-7.0460999999999996E-2</v>
+        <v>-3.9740000000000004E-2</v>
       </c>
       <c r="J27" s="11">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B23)/'YTD Calculation'!B23</f>
-        <v>-0.28410067526089627</v>
+        <v>-0.38293431553100066</v>
       </c>
       <c r="K27" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.18390482855143458</v>
+        <v>-0.29657102869139257</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -7090,7 +7090,7 @@
       </c>
       <c r="C28" s="6" cm="1">
         <f t="array" aca="1" ref="C28" ca="1">_FV(A28,"Price")</f>
-        <v>161.03</v>
+        <v>182.61</v>
       </c>
       <c r="D28" s="12">
         <v>142.16999999999999</v>
@@ -7104,23 +7104,23 @@
       </c>
       <c r="G28" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>23349.248060772319</v>
+        <v>26478.334399662381</v>
       </c>
       <c r="H28" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>2.1642984782752474E-2</v>
+        <v>2.3947966645059295E-2</v>
       </c>
       <c r="I28" s="15" cm="1">
         <f t="array" aca="1" ref="I28" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>1.3787000000000001E-2</v>
+        <v>6.0599999999999994E-3</v>
       </c>
       <c r="J28" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B24)/'YTD Calculation'!B24</f>
-        <v>-0.14853003384094757</v>
+        <v>-3.4422588832487264E-2</v>
       </c>
       <c r="K28" s="25">
         <f ca="1">(G28-E28)/E28</f>
-        <v>0.13265808539072954</v>
+        <v>0.2844481958219035</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -7133,7 +7133,7 @@
       </c>
       <c r="C29" s="41" cm="1">
         <f t="array" aca="1" ref="C29" ca="1">_FV(A29,"Price")</f>
-        <v>589.49</v>
+        <v>597.71</v>
       </c>
       <c r="D29" s="42">
         <v>229.7</v>
@@ -7147,23 +7147,23 @@
       </c>
       <c r="G29" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>316549.66280452767</v>
+        <v>320963.71262429259</v>
       </c>
       <c r="H29" s="46">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>0.29341756604890035</v>
+        <v>0.29029123086756409</v>
       </c>
       <c r="I29" s="15" cm="1">
         <f t="array" aca="1" ref="I29" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>1.4610000000000001E-3</v>
+        <v>-6.8289999999999991E-3</v>
       </c>
       <c r="J29" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B25)/'YTD Calculation'!B25</f>
-        <v>0.24720194647201954</v>
+        <v>0.26459325081984569</v>
       </c>
       <c r="K29" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>1.5663474096647803</v>
+        <v>1.6021332172398783</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -7176,7 +7176,7 @@
       </c>
       <c r="C30" s="6" cm="1">
         <f t="array" aca="1" ref="C30" ca="1">_FV(A30,"Price")</f>
-        <v>12.765000000000001</v>
+        <v>12.625</v>
       </c>
       <c r="D30" s="12">
         <v>20.47</v>
@@ -7190,23 +7190,23 @@
       </c>
       <c r="G30" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>12764.812921348317</v>
+        <v>12624.814973131413</v>
       </c>
       <c r="H30" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>1.1832014936513794E-2</v>
+        <v>1.1418340871186041E-2</v>
       </c>
       <c r="I30" s="15" cm="1">
         <f t="array" aca="1" ref="I30" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>-2.6316000000000003E-2</v>
+        <v>-3.8462000000000003E-2</v>
       </c>
       <c r="J30" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B26)/'YTD Calculation'!B26</f>
-        <v>-0.4462039045553145</v>
+        <v>-0.45227765726681129</v>
       </c>
       <c r="K30" s="25">
         <f ca="1">(G30-E30)/E30</f>
-        <v>-0.37640449438202239</v>
+        <v>-0.38324377137274052</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -7219,7 +7219,7 @@
       </c>
       <c r="C31" s="6" cm="1">
         <f t="array" aca="1" ref="C31" ca="1">_FV(A31,"Price")</f>
-        <v>183.74</v>
+        <v>186.07</v>
       </c>
       <c r="D31" s="12">
         <v>143.58000000000001</v>
@@ -7233,23 +7233,23 @@
       </c>
       <c r="G31" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>11943.394332079677</v>
+        <v>12094.848064493663</v>
       </c>
       <c r="H31" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>1.1070622107865111E-2</v>
+        <v>1.0939019564208218E-2</v>
       </c>
       <c r="I31" s="15" cm="1">
         <f t="array" aca="1" ref="I31" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>1.0949E-2</v>
+        <v>3.019E-3</v>
       </c>
       <c r="J31" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B27)/'YTD Calculation'!B27</f>
-        <v>0.15371091297249792</v>
+        <v>0.16834107748336058</v>
       </c>
       <c r="K31" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.27970469424710959</v>
+        <v>0.29593258113943449</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -7262,7 +7262,7 @@
       </c>
       <c r="C32" s="6" cm="1">
         <f t="array" aca="1" ref="C32" ca="1">_FV(A32,"Price")</f>
-        <v>102</v>
+        <v>101.17</v>
       </c>
       <c r="D32" s="12">
         <v>29.57</v>
@@ -7276,23 +7276,23 @@
       </c>
       <c r="G32" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>5606.6885356780522</v>
+        <v>5561.0654819073388</v>
       </c>
       <c r="H32" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>5.1969756946125449E-3</v>
+        <v>5.0296294571083614E-3</v>
       </c>
       <c r="I32" s="15" cm="1">
         <f t="array" aca="1" ref="I32" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>3.4429999999999999E-3</v>
+        <v>-2.1472000000000002E-2</v>
       </c>
       <c r="J32" s="11">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B28)/'YTD Calculation'!B28</f>
-        <v>0.25894840780054312</v>
+        <v>0.24870402369785247</v>
       </c>
       <c r="K32" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>2.449442002029083</v>
+        <v>2.4213730131890427</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -7305,7 +7305,7 @@
       </c>
       <c r="C33" s="6" cm="1">
         <f t="array" aca="1" ref="C33" ca="1">_FV(A33,"Price")</f>
-        <v>91.78</v>
+        <v>99.54</v>
       </c>
       <c r="D33" s="12">
         <v>23.4</v>
@@ -7319,23 +7319,23 @@
       </c>
       <c r="G33" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>51204.807222222218</v>
+        <v>55534.174230769233</v>
       </c>
       <c r="H33" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>4.7462978706204764E-2</v>
+        <v>5.02271227512079E-2</v>
       </c>
       <c r="I33" s="15" cm="1">
         <f t="array" aca="1" ref="I33" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>1.0682000000000001E-2</v>
+        <v>1.4058999999999999E-2</v>
       </c>
       <c r="J33" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B29)/'YTD Calculation'!B29</f>
-        <v>0.72856386815604157</v>
+        <v>0.87471396204241003</v>
       </c>
       <c r="K33" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9222222222222225</v>
+        <v>3.2538461538461538</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -7348,7 +7348,7 @@
       </c>
       <c r="C34" s="6" cm="1">
         <f t="array" aca="1" ref="C34" ca="1">_FV(A34,"Price")</f>
-        <v>15.8</v>
+        <v>16.364999999999998</v>
       </c>
       <c r="D34" s="12">
         <v>8.77</v>
@@ -7362,23 +7362,23 @@
       </c>
       <c r="G34" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>17054.271379703536</v>
+        <v>17664.123489167618</v>
       </c>
       <c r="H34" s="17">
         <f ca="1">Table1[[#This Row],[Total Value]]/Portfolio!$C$3</f>
-        <v>1.5808018099390815E-2</v>
+        <v>1.5976074391529264E-2</v>
       </c>
       <c r="I34" s="15" cm="1">
         <f t="array" aca="1" ref="I34" ca="1">_FV(Table1[[#This Row],[Stock]],"Change (%)",TRUE)</f>
-        <v>-7.5380000000000004E-3</v>
+        <v>2.7569999999999999E-3</v>
       </c>
       <c r="J34" s="15">
         <f ca="1">(Table1[[#This Row],[Live Price]]-'YTD Calculation'!B30)/'YTD Calculation'!B30</f>
-        <v>0.36915077989601403</v>
+        <v>0.41811091854419408</v>
       </c>
       <c r="K34" s="25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.80159635119726336</v>
+        <v>0.86602052451539335</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -7488,7 +7488,7 @@
       <c r="B3" s="71"/>
       <c r="C3" s="18">
         <f ca="1">SUM(Table1[Total Value])</f>
-        <v>1078836.7822251385</v>
+        <v>1105661.0689377724</v>
       </c>
       <c r="D3" s="21" t="e" vm="31">
         <f ca="1">SUMPRODUCT(H6:H34,Table1[Weight])</f>
@@ -7496,7 +7496,7 @@
       </c>
       <c r="E3" s="48">
         <f ca="1">SUMPRODUCT(Table2[Beta],Transaction!H6:H34)</f>
-        <v>0.9705950941387379</v>
+        <v>0.96831770157673624</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="22" customHeight="1"/>
@@ -7546,22 +7546,22 @@
       </c>
       <c r="E6" s="29" cm="1">
         <f t="array" aca="1" ref="E6" ca="1">_FV(A6,"Price")</f>
-        <v>242.7</v>
+        <v>228.01</v>
       </c>
       <c r="F6" s="49">
         <v>4.3E-3</v>
       </c>
       <c r="G6" s="30" cm="1">
         <f t="array" aca="1" ref="G6" ca="1">_FV(A6,"Market cap",TRUE)</f>
-        <v>3668609514000</v>
+        <v>3428784738700</v>
       </c>
       <c r="H6" s="31" cm="1">
         <f t="array" aca="1" ref="H6" ca="1">_FV(A6,"P/E",TRUE)</f>
-        <v>39.903300000000002</v>
+        <v>33.895400000000002</v>
       </c>
       <c r="I6" s="31" cm="1">
         <f t="array" aca="1" ref="I6" ca="1">_FV(A6,"Beta")</f>
-        <v>1.2093</v>
+        <v>1.1996</v>
       </c>
       <c r="J6" s="1"/>
     </row>
@@ -7582,22 +7582,22 @@
       </c>
       <c r="E7" s="29" cm="1">
         <f t="array" aca="1" ref="E7" ca="1">_FV(A7,"Price")</f>
-        <v>419.58</v>
+        <v>438.6</v>
       </c>
       <c r="F7" s="49">
         <v>0</v>
       </c>
       <c r="G7" s="30" cm="1">
         <f t="array" aca="1" ref="G7" ca="1">_FV(A7,"Market cap",TRUE)</f>
-        <v>184699116000</v>
+        <v>190926571260</v>
       </c>
       <c r="H7" s="31" cm="1">
         <f t="array" aca="1" ref="H7" ca="1">_FV(A7,"P/E",TRUE)</f>
-        <v>34.067999999999998</v>
+        <v>35.286999999999999</v>
       </c>
       <c r="I7" s="31" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">_FV(A7,"Beta")</f>
-        <v>1.3172999999999999</v>
+        <v>1.3126</v>
       </c>
       <c r="J7" s="1"/>
     </row>
@@ -7618,22 +7618,22 @@
       </c>
       <c r="E8" s="29" cm="1">
         <f t="array" aca="1" ref="E8" ca="1">_FV(A8,"Price")</f>
-        <v>291.89</v>
+        <v>307.32</v>
       </c>
       <c r="F8" s="51">
         <v>2.3900000000000001E-2</v>
       </c>
       <c r="G8" s="30" cm="1">
         <f t="array" aca="1" ref="G8" ca="1">_FV(A8,"Market cap",TRUE)</f>
-        <v>118932594541</v>
+        <v>123286000000</v>
       </c>
       <c r="H8" s="31" cm="1">
         <f t="array" aca="1" ref="H8" ca="1">_FV(A8,"P/E",TRUE)</f>
-        <v>31.1858</v>
+        <v>31.942</v>
       </c>
       <c r="I8" s="31" cm="1">
         <f t="array" aca="1" ref="I8" ca="1">_FV(A8,"Beta")</f>
-        <v>0.80500000000000005</v>
+        <v>0.80589999999999995</v>
       </c>
       <c r="J8" s="1"/>
     </row>
@@ -7654,22 +7654,22 @@
       </c>
       <c r="E9" s="29" cm="1">
         <f t="array" aca="1" ref="E9" ca="1">_FV(A9,"Price")</f>
-        <v>191.8</v>
+        <v>191.98</v>
       </c>
       <c r="F9" s="51">
         <v>2.3E-2</v>
       </c>
       <c r="G9" s="32" cm="1">
         <f t="array" aca="1" ref="G9" ca="1">_FV(A9,"Market cap",TRUE)</f>
-        <v>50696620000</v>
+        <v>50836975930</v>
       </c>
       <c r="H9" s="31" cm="1">
         <f t="array" aca="1" ref="H9" ca="1">_FV(A9,"P/E",TRUE)</f>
-        <v>12.3843</v>
+        <v>12.396000000000001</v>
       </c>
       <c r="I9" s="31" cm="1">
         <f t="array" aca="1" ref="I9" ca="1">_FV(A9,"Beta")</f>
-        <v>0.51900000000000002</v>
+        <v>0.51690000000000003</v>
       </c>
       <c r="J9" s="1"/>
     </row>
@@ -7690,22 +7690,22 @@
       </c>
       <c r="E10" s="29" cm="1">
         <f t="array" aca="1" ref="E10" ca="1">_FV(A10,"Price")</f>
-        <v>222.13</v>
+        <v>237.42</v>
       </c>
       <c r="F10" s="52">
         <v>0</v>
       </c>
       <c r="G10" s="33" cm="1">
         <f t="array" aca="1" ref="G10" ca="1">_FV(A10,"Market cap",TRUE)</f>
-        <v>2335699171300</v>
+        <v>2496473674200</v>
       </c>
       <c r="H10" s="31" cm="1">
         <f t="array" aca="1" ref="H10" ca="1">_FV(A10,"P/E",TRUE)</f>
-        <v>47.602600000000002</v>
+        <v>50.731900000000003</v>
       </c>
       <c r="I10" s="31" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">_FV(A10,"Beta")</f>
-        <v>1.1521999999999999</v>
+        <v>1.1567000000000001</v>
       </c>
       <c r="J10" s="1"/>
     </row>
@@ -7726,22 +7726,22 @@
       </c>
       <c r="E11" s="34" cm="1">
         <f t="array" aca="1" ref="E11" ca="1">_FV(A11,"Price")</f>
-        <v>440.15</v>
+        <v>450.15</v>
       </c>
       <c r="F11" s="52">
         <v>0</v>
       </c>
       <c r="G11" s="33" cm="1">
         <f t="array" aca="1" ref="G11" ca="1">_FV(A11,"Market cap",TRUE)</f>
-        <v>978680400000</v>
+        <v>1010430000000</v>
       </c>
       <c r="H11" s="31" cm="1">
         <f t="array" aca="1" ref="H11" ca="1">_FV(A11,"P/E",TRUE)</f>
-        <v>9.8800000000000008</v>
+        <v>10.1248</v>
       </c>
       <c r="I11" s="31" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">_FV(A11,"Beta")</f>
-        <v>0.88380000000000003</v>
+        <v>0.8841</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -7761,22 +7761,22 @@
       </c>
       <c r="E12" s="35" cm="1">
         <f t="array" aca="1" ref="E12" ca="1">_FV(A12,"Price")</f>
-        <v>361.07</v>
+        <v>361.51</v>
       </c>
       <c r="F12" s="51">
         <v>1.72E-2</v>
       </c>
       <c r="G12" s="33" cm="1">
         <f t="array" aca="1" ref="G12" ca="1">_FV(A12,"Market cap",TRUE)</f>
-        <v>175638700000</v>
+        <v>174537931775</v>
       </c>
       <c r="H12" s="31" cm="1">
         <f t="array" aca="1" ref="H12" ca="1">_FV(A12,"P/E",TRUE)</f>
-        <v>16.7454</v>
+        <v>16.3797</v>
       </c>
       <c r="I12" s="31" cm="1">
         <f t="array" aca="1" ref="I12" ca="1">_FV(A12,"Beta")</f>
-        <v>1.1082000000000001</v>
+        <v>1.1067</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -7796,22 +7796,22 @@
       </c>
       <c r="E13" s="35" cm="1">
         <f t="array" aca="1" ref="E13" ca="1">_FV(A13,"Price")</f>
-        <v>927.37</v>
+        <v>1005.83</v>
       </c>
       <c r="F13" s="51">
         <v>5.1999999999999998E-3</v>
       </c>
       <c r="G13" s="33" cm="1">
         <f t="array" aca="1" ref="G13" ca="1">_FV(A13,"Market cap",TRUE)</f>
-        <v>411658522893</v>
+        <v>446486830587</v>
       </c>
       <c r="H13" s="31" cm="1">
         <f t="array" aca="1" ref="H13" ca="1">_FV(A13,"P/E",TRUE)</f>
-        <v>54.103099999999998</v>
+        <v>57.538800000000002</v>
       </c>
       <c r="I13" s="31" cm="1">
         <f t="array" aca="1" ref="I13" ca="1">_FV(A13,"Beta")</f>
-        <v>0.83650000000000002</v>
+        <v>0.8397</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -7865,22 +7865,22 @@
       </c>
       <c r="E15" s="35" cm="1">
         <f t="array" aca="1" ref="E15" ca="1">_FV(A15,"Price")</f>
-        <v>71.62</v>
+        <v>71.47</v>
       </c>
       <c r="F15" s="51">
         <v>1.8499999999999999E-2</v>
       </c>
       <c r="G15" s="33" cm="1">
         <f t="array" aca="1" ref="G15" ca="1">_FV(A15,"Market cap",TRUE)</f>
-        <v>16421850000</v>
+        <v>15718089779</v>
       </c>
       <c r="H15" s="31" cm="1">
         <f t="array" aca="1" ref="H15" ca="1">_FV(A15,"P/E",TRUE)</f>
-        <v>11.7949</v>
+        <v>11.770200000000001</v>
       </c>
       <c r="I15" s="31" cm="1">
         <f t="array" aca="1" ref="I15" ca="1">_FV(A15,"Beta")</f>
-        <v>0.43819999999999998</v>
+        <v>0.43240000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -7900,22 +7900,22 @@
       </c>
       <c r="E16" s="35" cm="1">
         <f t="array" aca="1" ref="E16" ca="1">_FV(A16,"Price")</f>
-        <v>238.09</v>
+        <v>214.2</v>
       </c>
       <c r="F16" s="51">
         <v>4.4999999999999997E-3</v>
       </c>
       <c r="G16" s="33" cm="1">
         <f t="array" aca="1" ref="G16" ca="1">_FV(A16,"Market cap",TRUE)</f>
-        <v>169619100000</v>
+        <v>154031220000</v>
       </c>
       <c r="H16" s="31" cm="1">
         <f t="array" aca="1" ref="H16" ca="1">_FV(A16,"P/E",TRUE)</f>
-        <v>44.945500000000003</v>
+        <v>40.520600000000002</v>
       </c>
       <c r="I16" s="31" cm="1">
         <f t="array" aca="1" ref="I16" ca="1">_FV(A16,"Beta")</f>
-        <v>0.84099999999999997</v>
+        <v>0.83609999999999995</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -7935,22 +7935,22 @@
       </c>
       <c r="E17" s="35" cm="1">
         <f t="array" aca="1" ref="E17" ca="1">_FV(A17,"Price")</f>
-        <v>109.76</v>
+        <v>114.06</v>
       </c>
       <c r="F17" s="51">
         <v>9.2999999999999992E-3</v>
       </c>
       <c r="G17" s="33" cm="1">
         <f t="array" aca="1" ref="G17" ca="1">_FV(A17,"Market cap",TRUE)</f>
-        <v>201304000000</v>
+        <v>206272947600</v>
       </c>
       <c r="H17" s="31" cm="1">
         <f t="array" aca="1" ref="H17" ca="1">_FV(A17,"P/E",TRUE)</f>
-        <v>40.406399999999998</v>
+        <v>41.989400000000003</v>
       </c>
       <c r="I17" s="31" cm="1">
         <f t="array" aca="1" ref="I17" ca="1">_FV(A17,"Beta")</f>
-        <v>1.4280999999999999</v>
+        <v>1.4273</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -7970,22 +7970,22 @@
       </c>
       <c r="E18" s="35" cm="1">
         <f t="array" aca="1" ref="E18" ca="1">_FV(A18,"Price")</f>
-        <v>195.39</v>
+        <v>202.64</v>
       </c>
       <c r="F18" s="51">
         <v>4.1999999999999997E-3</v>
       </c>
       <c r="G18" s="33" cm="1">
         <f t="array" aca="1" ref="G18" ca="1">_FV(A18,"Market cap",TRUE)</f>
-        <v>2399745000000</v>
+        <v>2506153000000</v>
       </c>
       <c r="H18" s="31" cm="1">
         <f t="array" aca="1" ref="H18" ca="1">_FV(A18,"P/E",TRUE)</f>
-        <v>26.080500000000001</v>
+        <v>26.866800000000001</v>
       </c>
       <c r="I18" s="31" cm="1">
         <f t="array" aca="1" ref="I18" ca="1">_FV(A18,"Beta")</f>
-        <v>0.9869</v>
+        <v>0.99099999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -8005,22 +8005,22 @@
       </c>
       <c r="E19" s="35" cm="1">
         <f t="array" aca="1" ref="E19" ca="1">_FV(A19,"Price")</f>
-        <v>387.2</v>
+        <v>408.82</v>
       </c>
       <c r="F19" s="51">
         <v>2.6100000000000002E-2</v>
       </c>
       <c r="G19" s="33" cm="1">
         <f t="array" aca="1" ref="G19" ca="1">_FV(A19,"Market cap",TRUE)</f>
-        <v>386596900000</v>
+        <v>406106498132</v>
       </c>
       <c r="H19" s="31" cm="1">
         <f t="array" aca="1" ref="H19" ca="1">_FV(A19,"P/E",TRUE)</f>
-        <v>26.302</v>
+        <v>27.770600000000002</v>
       </c>
       <c r="I19" s="31" cm="1">
         <f t="array" aca="1" ref="I19" ca="1">_FV(A19,"Beta")</f>
-        <v>1.0556000000000001</v>
+        <v>1.0584</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -8040,22 +8040,22 @@
       </c>
       <c r="E20" s="35" cm="1">
         <f t="array" aca="1" ref="E20" ca="1">_FV(A20,"Price")</f>
-        <v>220.17</v>
+        <v>222.41</v>
       </c>
       <c r="F20" s="51">
         <v>2.01E-2</v>
       </c>
       <c r="G20" s="33" cm="1">
         <f t="array" aca="1" ref="G20" ca="1">_FV(A20,"Market cap",TRUE)</f>
-        <v>143164970058</v>
+        <v>144621524234</v>
       </c>
       <c r="H20" s="31" cm="1">
         <f t="array" aca="1" ref="H20" ca="1">_FV(A20,"P/E",TRUE)</f>
-        <v>25.484300000000001</v>
+        <v>25.675999999999998</v>
       </c>
       <c r="I20" s="31" cm="1">
         <f t="array" aca="1" ref="I20" ca="1">_FV(A20,"Beta")</f>
-        <v>1.0485</v>
+        <v>1.0452999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -8075,22 +8075,22 @@
       </c>
       <c r="E21" s="35" cm="1">
         <f t="array" aca="1" ref="E21" ca="1">_FV(A21,"Price")</f>
-        <v>142.27000000000001</v>
+        <v>151.87</v>
       </c>
       <c r="F21" s="51">
         <v>3.32E-2</v>
       </c>
       <c r="G21" s="33" cm="1">
         <f t="array" aca="1" ref="G21" ca="1">_FV(A21,"Market cap",TRUE)</f>
-        <v>347155200000</v>
+        <v>365645705010</v>
       </c>
       <c r="H21" s="31" cm="1">
         <f t="array" aca="1" ref="H21" ca="1">_FV(A21,"P/E",TRUE)</f>
-        <v>23.3874</v>
+        <v>26.196200000000001</v>
       </c>
       <c r="I21" s="31" cm="1">
         <f t="array" aca="1" ref="I21" ca="1">_FV(A21,"Beta")</f>
-        <v>0.50700000000000001</v>
+        <v>0.5111</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -8110,22 +8110,22 @@
       </c>
       <c r="E22" s="35" cm="1">
         <f t="array" aca="1" ref="E22" ca="1">_FV(A22,"Price")</f>
-        <v>468.85</v>
+        <v>455.4</v>
       </c>
       <c r="F22" s="51">
         <v>2.7300000000000001E-2</v>
       </c>
       <c r="G22" s="33" cm="1">
         <f t="array" aca="1" ref="G22" ca="1">_FV(A22,"Market cap",TRUE)</f>
-        <v>114208300000</v>
+        <v>107194738860</v>
       </c>
       <c r="H22" s="31" cm="1">
         <f t="array" aca="1" ref="H22" ca="1">_FV(A22,"P/E",TRUE)</f>
-        <v>16.958600000000001</v>
+        <v>20.450199999999999</v>
       </c>
       <c r="I22" s="31" cm="1">
         <f t="array" aca="1" ref="I22" ca="1">_FV(A22,"Beta")</f>
-        <v>0.4879</v>
+        <v>0.48230000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -8145,22 +8145,22 @@
       </c>
       <c r="E23" s="35" cm="1">
         <f t="array" aca="1" ref="E23" ca="1">_FV(A23,"Price")</f>
-        <v>516.4</v>
+        <v>564.34100000000001</v>
       </c>
       <c r="F23" s="51">
         <v>6.1000000000000004E-3</v>
       </c>
       <c r="G23" s="33" cm="1">
         <f t="array" aca="1" ref="G23" ca="1">_FV(A23,"Market cap",TRUE)</f>
-        <v>478520400000</v>
+        <v>515807674000</v>
       </c>
       <c r="H23" s="31" cm="1">
         <f t="array" aca="1" ref="H23" ca="1">_FV(A23,"P/E",TRUE)</f>
-        <v>39.033099999999997</v>
+        <v>40.626100000000001</v>
       </c>
       <c r="I23" s="31" cm="1">
         <f t="array" aca="1" ref="I23" ca="1">_FV(A23,"Beta")</f>
-        <v>1.101</v>
+        <v>1.1032</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -8180,22 +8180,22 @@
       </c>
       <c r="E24" s="35" cm="1">
         <f t="array" aca="1" ref="E24" ca="1">_FV(A24,"Price")</f>
-        <v>424.56</v>
+        <v>410.92</v>
       </c>
       <c r="F24" s="51">
         <v>6.4000000000000003E-3</v>
       </c>
       <c r="G24" s="33" cm="1">
         <f t="array" aca="1" ref="G24" ca="1">_FV(A24,"Market cap",TRUE)</f>
-        <v>3156553077360</v>
+        <v>3054771883440</v>
       </c>
       <c r="H24" s="31" cm="1">
         <f t="array" aca="1" ref="H24" ca="1">_FV(A24,"P/E",TRUE)</f>
-        <v>34.933300000000003</v>
+        <v>33.100299999999997</v>
       </c>
       <c r="I24" s="31" cm="1">
         <f t="array" aca="1" ref="I24" ca="1">_FV(A24,"Beta")</f>
-        <v>0.89910000000000001</v>
+        <v>0.89470000000000005</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -8215,22 +8215,22 @@
       </c>
       <c r="E25" s="35" cm="1">
         <f t="array" aca="1" ref="E25" ca="1">_FV(A25,"Price")</f>
-        <v>70.66</v>
+        <v>71.069999999999993</v>
       </c>
       <c r="F25" s="51">
         <v>2.8299999999999999E-2</v>
       </c>
       <c r="G25" s="33" cm="1">
         <f t="array" aca="1" ref="G25" ca="1">_FV(A25,"Market cap",TRUE)</f>
-        <v>148040600000</v>
+        <v>146148703350</v>
       </c>
       <c r="H25" s="31" cm="1">
         <f t="array" aca="1" ref="H25" ca="1">_FV(A25,"P/E",TRUE)</f>
-        <v>20.956199999999999</v>
+        <v>21.0671</v>
       </c>
       <c r="I25" s="31" cm="1">
         <f t="array" aca="1" ref="I25" ca="1">_FV(A25,"Beta")</f>
-        <v>0.57820000000000005</v>
+        <v>0.57679999999999998</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -8250,22 +8250,22 @@
       </c>
       <c r="E26" s="35" cm="1">
         <f t="array" aca="1" ref="E26" ca="1">_FV(A26,"Price")</f>
-        <v>69.14</v>
+        <v>74.31</v>
       </c>
       <c r="F26" s="51">
         <v>2.0400000000000001E-2</v>
       </c>
       <c r="G26" s="33" cm="1">
         <f t="array" aca="1" ref="G26" ca="1">_FV(A26,"Market cap",TRUE)</f>
-        <v>109121600000</v>
+        <v>113744900000</v>
       </c>
       <c r="H26" s="31" cm="1">
         <f t="array" aca="1" ref="H26" ca="1">_FV(A26,"P/E",TRUE)</f>
-        <v>22.68</v>
+        <v>24.53</v>
       </c>
       <c r="I26" s="31" cm="1">
         <f t="array" aca="1" ref="I26" ca="1">_FV(A26,"Beta")</f>
-        <v>1.0154000000000001</v>
+        <v>1.0152000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -8285,22 +8285,22 @@
       </c>
       <c r="E27" s="35" cm="1">
         <f t="array" aca="1" ref="E27" ca="1">_FV(A27,"Price")</f>
-        <v>58.31</v>
+        <v>50.26</v>
       </c>
       <c r="F27" s="51">
         <v>0</v>
       </c>
       <c r="G27" s="33" cm="1">
         <f t="array" aca="1" ref="G27" ca="1">_FV(A27,"Market cap",TRUE)</f>
-        <v>24828252225</v>
+        <v>21400582350</v>
       </c>
       <c r="H27" s="31" cm="1">
         <f t="array" aca="1" ref="H27" ca="1">_FV(A27,"P/E",TRUE)</f>
-        <v>14.596399999999999</v>
+        <v>12.4712</v>
       </c>
       <c r="I27" s="31" cm="1">
         <f t="array" aca="1" ref="I27" ca="1">_FV(A27,"Beta")</f>
-        <v>1.6337999999999999</v>
+        <v>1.6129</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -8320,21 +8320,21 @@
       </c>
       <c r="E28" s="35" cm="1">
         <f t="array" aca="1" ref="E28" ca="1">_FV(A28,"Price")</f>
-        <v>161.03</v>
+        <v>182.61</v>
       </c>
       <c r="F28" s="51">
         <v>0</v>
       </c>
       <c r="G28" s="33" cm="1">
         <f t="array" aca="1" ref="G28" ca="1">_FV(A28,"Market cap",TRUE)</f>
-        <v>53548820000</v>
+        <v>60279561000</v>
       </c>
       <c r="H28" s="28">
         <v>0</v>
       </c>
       <c r="I28" s="31" cm="1">
         <f t="array" aca="1" ref="I28" ca="1">_FV(A28,"Beta")</f>
-        <v>1.0516000000000001</v>
+        <v>1.0732999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -8354,21 +8354,21 @@
       </c>
       <c r="E29" s="37" cm="1">
         <f t="array" aca="1" ref="E29" ca="1">_FV(A29,"Price")</f>
-        <v>589.49</v>
+        <v>597.71</v>
       </c>
       <c r="F29" s="53">
         <v>1.26E-2</v>
       </c>
       <c r="G29" s="38" cm="1">
         <f t="array" aca="1" ref="G29" ca="1">_FV(A29,"Market cap",TRUE)</f>
-        <v>623795251613.90002</v>
+        <v>627680565767.93005</v>
       </c>
       <c r="H29" s="36">
         <v>0</v>
       </c>
       <c r="I29" s="39" cm="1">
         <f t="array" aca="1" ref="I29" ca="1">_FV(A29,"Beta")</f>
-        <v>0.99829999999999997</v>
+        <v>0.99819999999999998</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -8388,22 +8388,22 @@
       </c>
       <c r="E30" s="35" cm="1">
         <f t="array" aca="1" ref="E30" ca="1">_FV(A30,"Price")</f>
-        <v>12.765000000000001</v>
+        <v>12.625</v>
       </c>
       <c r="F30" s="51">
         <v>8.2699999999999996E-2</v>
       </c>
       <c r="G30" s="40" cm="1">
         <f t="array" aca="1" ref="G30" ca="1">_FV(A30,"Market cap",TRUE)</f>
-        <v>35262590000</v>
+        <v>37538910000</v>
       </c>
       <c r="H30" s="31" cm="1">
         <f t="array" aca="1" ref="H30" ca="1">_FV(A30,"P/E",TRUE)</f>
-        <v>2.7031000000000001</v>
+        <v>2.6734</v>
       </c>
       <c r="I30" s="31" cm="1">
         <f t="array" aca="1" ref="I30" ca="1">_FV(A30,"Beta")</f>
-        <v>1.5183</v>
+        <v>1.4999</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -8423,14 +8423,14 @@
       </c>
       <c r="E31" s="35" cm="1">
         <f t="array" aca="1" ref="E31" ca="1">_FV(A31,"Price")</f>
-        <v>183.74</v>
+        <v>186.07</v>
       </c>
       <c r="F31" s="51">
         <v>0</v>
       </c>
       <c r="G31" s="33" cm="1">
         <f t="array" aca="1" ref="G31" ca="1">_FV(A31,"Market cap",TRUE)</f>
-        <v>32269778476</v>
+        <v>32678990318</v>
       </c>
       <c r="H31" s="31" cm="1">
         <f t="array" aca="1" ref="H31" ca="1">_FV(A31,"P/E",TRUE)</f>
@@ -8438,7 +8438,7 @@
       </c>
       <c r="I31" s="31" cm="1">
         <f t="array" aca="1" ref="I31" ca="1">_FV(A31,"Beta")</f>
-        <v>0.88900000000000001</v>
+        <v>0.88739999999999997</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -8458,22 +8458,22 @@
       </c>
       <c r="E32" s="35" cm="1">
         <f t="array" aca="1" ref="E32" ca="1">_FV(A32,"Price")</f>
-        <v>102</v>
+        <v>101.17</v>
       </c>
       <c r="F32" s="51">
         <v>3.8E-3</v>
       </c>
       <c r="G32" s="33" cm="1">
         <f t="array" aca="1" ref="G32" ca="1">_FV(A32,"Market cap",TRUE)</f>
-        <v>24928620000</v>
+        <v>25020130126</v>
       </c>
       <c r="H32" s="31" cm="1">
         <f t="array" aca="1" ref="H32" ca="1">_FV(A32,"P/E",TRUE)</f>
-        <v>31.476600000000001</v>
+        <v>31.220500000000001</v>
       </c>
       <c r="I32" s="31" cm="1">
         <f t="array" aca="1" ref="I32" ca="1">_FV(A32,"Beta")</f>
-        <v>0.78800000000000003</v>
+        <v>0.77900000000000003</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -8493,22 +8493,22 @@
       </c>
       <c r="E33" s="35" cm="1">
         <f t="array" aca="1" ref="E33" ca="1">_FV(A33,"Price")</f>
-        <v>91.78</v>
+        <v>99.54</v>
       </c>
       <c r="F33" s="51">
         <v>1.18E-2</v>
       </c>
       <c r="G33" s="33" cm="1">
         <f t="array" aca="1" ref="G33" ca="1">_FV(A33,"Market cap",TRUE)</f>
-        <v>729270800000</v>
+        <v>799643242440</v>
       </c>
       <c r="H33" s="31" cm="1">
         <f t="array" aca="1" ref="H33" ca="1">_FV(A33,"P/E",TRUE)</f>
-        <v>46.339500000000001</v>
+        <v>50.2575</v>
       </c>
       <c r="I33" s="31" cm="1">
         <f t="array" aca="1" ref="I33" ca="1">_FV(A33,"Beta")</f>
-        <v>0.5464</v>
+        <v>0.55210000000000004</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -8528,21 +8528,21 @@
       </c>
       <c r="E34" s="35" cm="1">
         <f t="array" aca="1" ref="E34" ca="1">_FV(A34,"Price")</f>
-        <v>15.8</v>
+        <v>16.364999999999998</v>
       </c>
       <c r="F34" s="51">
         <v>0</v>
       </c>
       <c r="G34" s="33" cm="1">
         <f t="array" aca="1" ref="G34" ca="1">_FV(A34,"Market cap",TRUE)</f>
-        <v>1160699000</v>
+        <v>1187624000</v>
       </c>
       <c r="H34" s="28">
         <v>0</v>
       </c>
       <c r="I34" s="31" cm="1">
         <f t="array" aca="1" ref="I34" ca="1">_FV(A34,"Beta")</f>
-        <v>1.6990000000000001</v>
+        <v>1.631</v>
       </c>
     </row>
     <row r="69" spans="2:2">

</xml_diff>